<commit_message>
Atualizacao da serie historica.
</commit_message>
<xml_diff>
--- a/Database/Serie de Equity Risk Premium.xlsx
+++ b/Database/Serie de Equity Risk Premium.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\ERP\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42A1FC24-1D46-402A-B5C2-4C486FF094EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48BB9243-AB5E-4597-B179-C2B767B6BCFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -263,10 +263,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Planilha1!$A$2:$A$338</c:f>
+              <c:f>Planilha1!$A$2:$A$339</c:f>
               <c:numCache>
                 <c:formatCode>mmm\-yy</c:formatCode>
-                <c:ptCount val="337"/>
+                <c:ptCount val="338"/>
                 <c:pt idx="0">
                   <c:v>34700</c:v>
                 </c:pt>
@@ -1277,16 +1277,19 @@
                 </c:pt>
                 <c:pt idx="336">
                   <c:v>44927</c:v>
+                </c:pt>
+                <c:pt idx="337">
+                  <c:v>44958</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Planilha1!$B$2:$B$338</c:f>
+              <c:f>Planilha1!$B$2:$B$339</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="337"/>
+                <c:ptCount val="338"/>
                 <c:pt idx="0">
                   <c:v>3.5906071097335332E-2</c:v>
                 </c:pt>
@@ -2297,6 +2300,9 @@
                 </c:pt>
                 <c:pt idx="336">
                   <c:v>0.112566</c:v>
+                </c:pt>
+                <c:pt idx="337">
+                  <c:v>0.10406600000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3330,10 +3336,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:RX338"/>
+  <dimension ref="A1:RX339"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W13" sqref="W13"/>
+      <selection activeCell="X20" sqref="X20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16672,6 +16678,14 @@
         <v>0.112566</v>
       </c>
     </row>
+    <row r="339" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A339" s="10">
+        <v>44958</v>
+      </c>
+      <c r="B339" s="9">
+        <v>0.10406600000000001</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -16680,21 +16694,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100FF602FB71C72A040B83BAD34EB50244A" ma:contentTypeVersion="13" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="ecb216dc5589f7bce5d8d0d60e90dc0d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="807d706a-80d8-4f03-8ed4-ece1162c7e44" xmlns:ns4="ea144f7f-7cb8-4e40-aa15-78233897bd5c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8b5314697a99cd150715f13355001d93" ns3:_="" ns4:_="">
     <xsd:import namespace="807d706a-80d8-4f03-8ed4-ece1162c7e44"/>
@@ -16917,10 +16916,36 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1EB3165A-A967-440B-92EF-0ADCFAB0BB15}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E376484F-D910-4B39-9F72-4143D5D135A3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="807d706a-80d8-4f03-8ed4-ece1162c7e44"/>
+    <ds:schemaRef ds:uri="ea144f7f-7cb8-4e40-aa15-78233897bd5c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -16943,20 +16968,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E376484F-D910-4B39-9F72-4143D5D135A3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1EB3165A-A967-440B-92EF-0ADCFAB0BB15}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="807d706a-80d8-4f03-8ed4-ece1162c7e44"/>
-    <ds:schemaRef ds:uri="ea144f7f-7cb8-4e40-aa15-78233897bd5c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
adicao de dataset 2023-06-03
</commit_message>
<xml_diff>
--- a/Database/Serie de Equity Risk Premium.xlsx
+++ b/Database/Serie de Equity Risk Premium.xlsx
@@ -1,24 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bteba\Documents\GitHub\ERP\Database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Teo\Documents\GitHub\ERP\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2065071-B52D-41A3-A6BA-9F61DEC484C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF790E72-BD4D-41BA-B88E-BFB8C578A051}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -97,7 +108,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="17" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -112,6 +123,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1261,6 +1273,9 @@
                 <c:pt idx="339">
                   <c:v>45017</c:v>
                 </c:pt>
+                <c:pt idx="340">
+                  <c:v>45047</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -2289,6 +2304,9 @@
                 </c:pt>
                 <c:pt idx="339">
                   <c:v>9.7161250237506505E-2</c:v>
+                </c:pt>
+                <c:pt idx="340">
+                  <c:v>8.9197844933858697E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3370,23 +3388,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:RX342"/>
+  <dimension ref="A1:RX343"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" topLeftCell="A310" workbookViewId="0">
+      <selection activeCell="B343" sqref="B343"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="6" customWidth="1"/>
+    <col min="1" max="2" width="11.42578125" customWidth="1"/>
     <col min="5" max="5" width="12.42578125" customWidth="1"/>
     <col min="40" max="40" width="9" customWidth="1"/>
     <col min="498" max="498" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A1"/>
       <c r="B1" t="s">
         <v>2</v>
       </c>
@@ -16432,7 +16448,7 @@
         <v>9.3984258626188408E-2</v>
       </c>
     </row>
-    <row r="305" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A305" s="5">
         <v>43891</v>
       </c>
@@ -16440,7 +16456,7 @@
         <v>0.11444455602995118</v>
       </c>
     </row>
-    <row r="306" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A306" s="5">
         <v>43922</v>
       </c>
@@ -16448,7 +16464,7 @@
         <v>0.11883485001315314</v>
       </c>
     </row>
-    <row r="307" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A307" s="5">
         <v>43952</v>
       </c>
@@ -16456,7 +16472,7 @@
         <v>0.10802006518576782</v>
       </c>
     </row>
-    <row r="308" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A308" s="5">
         <v>43983</v>
       </c>
@@ -16464,7 +16480,7 @@
         <v>0.10150000000000001</v>
       </c>
     </row>
-    <row r="309" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A309" s="5">
         <v>44013</v>
       </c>
@@ -16472,7 +16488,7 @@
         <v>0.10394071190796175</v>
       </c>
     </row>
-    <row r="310" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A310" s="5">
         <v>44044</v>
       </c>
@@ -16480,7 +16496,7 @@
         <v>9.8747906968658955E-2</v>
       </c>
     </row>
-    <row r="311" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A311" s="5">
         <v>44075</v>
       </c>
@@ -16488,7 +16504,7 @@
         <v>0.10280377344670942</v>
       </c>
     </row>
-    <row r="312" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A312" s="5">
         <v>44105</v>
       </c>
@@ -16496,7 +16512,7 @@
         <v>0.1003081555378784</v>
       </c>
     </row>
-    <row r="313" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A313" s="5">
         <v>44136</v>
       </c>
@@ -16504,237 +16520,275 @@
         <v>9.4781090636132159E-2</v>
       </c>
     </row>
-    <row r="314" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A314" s="5">
         <v>44166</v>
       </c>
       <c r="B314" s="6">
         <v>9.9688114787269883E-2</v>
       </c>
-    </row>
-    <row r="315" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C314" s="8"/>
+    </row>
+    <row r="315" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A315" s="5">
         <v>44197</v>
       </c>
       <c r="B315" s="6">
         <v>0.10345953791176479</v>
       </c>
-    </row>
-    <row r="316" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C315" s="8"/>
+    </row>
+    <row r="316" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A316" s="5">
         <v>44228</v>
       </c>
       <c r="B316" s="6">
         <v>9.9036976535253174E-2</v>
       </c>
-    </row>
-    <row r="317" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C316" s="8"/>
+    </row>
+    <row r="317" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A317" s="5">
         <v>44256</v>
       </c>
       <c r="B317" s="6">
         <v>0.11202004609682872</v>
       </c>
-    </row>
-    <row r="318" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C317" s="8"/>
+    </row>
+    <row r="318" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A318" s="5">
         <v>44287</v>
       </c>
       <c r="B318" s="6">
         <v>0.1105</v>
       </c>
-    </row>
-    <row r="319" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C318" s="8"/>
+    </row>
+    <row r="319" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A319" s="5">
         <v>44317</v>
       </c>
       <c r="B319" s="6">
         <v>0.103756060197642</v>
       </c>
-    </row>
-    <row r="320" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C319" s="8"/>
+    </row>
+    <row r="320" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A320" s="5">
         <v>44348</v>
       </c>
       <c r="B320" s="6">
         <v>0.11288777024068533</v>
       </c>
-    </row>
-    <row r="321" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C320" s="8"/>
+    </row>
+    <row r="321" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A321" s="5">
         <v>44378</v>
       </c>
       <c r="B321" s="6">
         <v>0.1217</v>
       </c>
-    </row>
-    <row r="322" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C321" s="8"/>
+    </row>
+    <row r="322" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A322" s="5">
         <v>44409</v>
       </c>
       <c r="B322" s="6">
         <v>0.11860470570232673</v>
       </c>
-    </row>
-    <row r="323" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C322" s="8"/>
+    </row>
+    <row r="323" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A323" s="5">
         <v>44440</v>
       </c>
       <c r="B323" s="6">
         <v>0.15321467349306883</v>
       </c>
-    </row>
-    <row r="324" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C323" s="8"/>
+    </row>
+    <row r="324" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A324" s="5">
         <v>44470</v>
       </c>
       <c r="B324" s="6">
         <v>0.1565</v>
       </c>
-    </row>
-    <row r="325" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C324" s="8"/>
+    </row>
+    <row r="325" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A325" s="5">
         <v>44501</v>
       </c>
       <c r="B325" s="6">
         <v>0.15480116295464194</v>
       </c>
-    </row>
-    <row r="326" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C325" s="8"/>
+    </row>
+    <row r="326" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A326" s="5">
         <v>44531</v>
       </c>
       <c r="B326" s="6">
         <v>0.18086975473681763</v>
       </c>
-    </row>
-    <row r="327" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C326" s="8"/>
+    </row>
+    <row r="327" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A327" s="5">
         <v>44562</v>
       </c>
       <c r="B327" s="6">
         <v>0.15203711549166959</v>
       </c>
-    </row>
-    <row r="328" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C327" s="8"/>
+    </row>
+    <row r="328" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A328" s="5">
         <v>44593</v>
       </c>
       <c r="B328" s="6">
         <v>0.15045086518646858</v>
       </c>
-    </row>
-    <row r="329" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C328" s="8"/>
+    </row>
+    <row r="329" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A329" s="5">
         <v>44621</v>
       </c>
       <c r="B329" s="6">
         <v>0.13402699778646815</v>
       </c>
-    </row>
-    <row r="330" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C329" s="8"/>
+    </row>
+    <row r="330" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A330" s="5">
         <v>44652</v>
       </c>
       <c r="B330" s="6">
         <v>0.13661550466927599</v>
       </c>
-    </row>
-    <row r="331" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C330" s="8"/>
+    </row>
+    <row r="331" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A331" s="5">
         <v>44682</v>
       </c>
       <c r="B331" s="6">
         <v>0.1321</v>
       </c>
-    </row>
-    <row r="332" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C331" s="8"/>
+    </row>
+    <row r="332" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A332" s="5">
         <v>44713</v>
       </c>
       <c r="B332" s="6">
         <v>0.16510000000000002</v>
       </c>
-    </row>
-    <row r="333" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C332" s="8"/>
+    </row>
+    <row r="333" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A333" s="5">
         <v>44743</v>
       </c>
       <c r="B333" s="6">
         <v>0.1585</v>
       </c>
-    </row>
-    <row r="334" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C333" s="8"/>
+    </row>
+    <row r="334" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A334" s="5">
         <v>44774</v>
       </c>
       <c r="B334" s="6">
         <v>0.1331</v>
       </c>
-    </row>
-    <row r="335" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C334" s="8"/>
+    </row>
+    <row r="335" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A335" s="5">
         <v>44805</v>
       </c>
       <c r="B335" s="6">
         <v>0.14630000000000001</v>
       </c>
-    </row>
-    <row r="336" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C335" s="8"/>
+    </row>
+    <row r="336" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A336" s="5">
         <v>44835</v>
       </c>
       <c r="B336" s="6">
         <v>0.1197</v>
       </c>
-    </row>
-    <row r="337" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C336" s="8"/>
+    </row>
+    <row r="337" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A337" s="5">
         <v>44866</v>
       </c>
       <c r="B337" s="6">
         <v>0.1177</v>
       </c>
-    </row>
-    <row r="338" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C337" s="8"/>
+    </row>
+    <row r="338" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A338" s="5">
         <v>44896</v>
       </c>
       <c r="B338" s="6">
         <v>0.1172183756433729</v>
       </c>
-    </row>
-    <row r="339" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C338" s="8"/>
+    </row>
+    <row r="339" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A339" s="5">
         <v>44927</v>
       </c>
       <c r="B339" s="6">
         <v>0.112566</v>
       </c>
-    </row>
-    <row r="340" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C339" s="8"/>
+    </row>
+    <row r="340" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A340" s="5">
         <v>44958</v>
       </c>
       <c r="B340" s="6">
         <v>0.10406600000000001</v>
       </c>
-    </row>
-    <row r="341" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C340" s="8"/>
+    </row>
+    <row r="341" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A341" s="5">
         <v>44986</v>
       </c>
       <c r="B341" s="6">
         <v>0.100060632666334</v>
       </c>
-    </row>
-    <row r="342" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C341" s="8"/>
+    </row>
+    <row r="342" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A342" s="5">
         <v>45017</v>
       </c>
       <c r="B342" s="6">
         <v>9.7161250237506505E-2</v>
       </c>
+      <c r="C342" s="8"/>
+    </row>
+    <row r="343" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A343" s="5">
+        <v>45047</v>
+      </c>
+      <c r="B343" s="6">
+        <v>8.9197844933858697E-2</v>
+      </c>
+      <c r="C343" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Atualizacao do ERP 2023-08
</commit_message>
<xml_diff>
--- a/Database/Serie de Equity Risk Premium.xlsx
+++ b/Database/Serie de Equity Risk Premium.xlsx
@@ -5,20 +5,31 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Teo\Documents\GitHub\ERP\Database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bteba\Documents\GitHub\ERP\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1774068A-2CCD-4CC3-ADF5-4F1E31B5447B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1D2A86A-69FD-4C76-86D4-BDCEADF9BB64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -98,7 +109,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="17" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -115,6 +126,7 @@
     </xf>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1273,6 +1285,9 @@
                 <c:pt idx="342">
                   <c:v>45108</c:v>
                 </c:pt>
+                <c:pt idx="343">
+                  <c:v>45139</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -2310,6 +2325,9 @@
                 </c:pt>
                 <c:pt idx="342">
                   <c:v>7.9421854001553702E-2</c:v>
+                </c:pt>
+                <c:pt idx="343">
+                  <c:v>8.8703735811575105E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3393,8 +3411,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:RX349"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A343" sqref="A343:B343"/>
+    <sheetView tabSelected="1" topLeftCell="A313" workbookViewId="0">
+      <selection activeCell="D346" sqref="D346"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16730,7 +16748,7 @@
       </c>
       <c r="C336" s="8"/>
     </row>
-    <row r="337" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A337" s="5">
         <v>44866</v>
       </c>
@@ -16739,7 +16757,7 @@
       </c>
       <c r="C337" s="8"/>
     </row>
-    <row r="338" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A338" s="5">
         <v>44896</v>
       </c>
@@ -16748,7 +16766,7 @@
       </c>
       <c r="C338" s="8"/>
     </row>
-    <row r="339" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A339" s="5">
         <v>44927</v>
       </c>
@@ -16757,7 +16775,7 @@
       </c>
       <c r="C339" s="8"/>
     </row>
-    <row r="340" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A340" s="5">
         <v>44958</v>
       </c>
@@ -16766,7 +16784,7 @@
       </c>
       <c r="C340" s="8"/>
     </row>
-    <row r="341" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A341" s="5">
         <v>44986</v>
       </c>
@@ -16775,7 +16793,7 @@
       </c>
       <c r="C341" s="8"/>
     </row>
-    <row r="342" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A342" s="5">
         <v>45017</v>
       </c>
@@ -16784,7 +16802,7 @@
       </c>
       <c r="C342" s="8"/>
     </row>
-    <row r="343" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A343" s="5">
         <v>45047</v>
       </c>
@@ -16792,7 +16810,7 @@
         <v>9.6838061660370997E-2</v>
       </c>
     </row>
-    <row r="344" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A344" s="5">
         <v>45078</v>
       </c>
@@ -16801,7 +16819,7 @@
       </c>
       <c r="C344" s="8"/>
     </row>
-    <row r="345" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A345" s="5">
         <v>45108</v>
       </c>
@@ -16809,21 +16827,27 @@
         <v>7.9421854001553702E-2</v>
       </c>
     </row>
-    <row r="346" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A346" s="9"/>
-    </row>
-    <row r="347" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A346" s="5">
+        <v>45139</v>
+      </c>
+      <c r="B346" s="6">
+        <v>8.8703735811575105E-2</v>
+      </c>
+      <c r="D346" s="10"/>
+    </row>
+    <row r="347" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A347" s="9"/>
     </row>
-    <row r="348" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A348" s="9"/>
     </row>
-    <row r="349" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A349" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Atualizacao da base de dados
</commit_message>
<xml_diff>
--- a/Database/Serie de Equity Risk Premium.xlsx
+++ b/Database/Serie de Equity Risk Premium.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bteba\Documents\GitHub\ERP\Database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bteba\Documents\Github\ERP\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1D2A86A-69FD-4C76-86D4-BDCEADF9BB64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98482026-E023-4AD6-8E48-410CAAA5D3B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$2:$B$2</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -112,6 +115,8 @@
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="17" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -124,8 +129,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1288,6 +1291,12 @@
                 <c:pt idx="343">
                   <c:v>45139</c:v>
                 </c:pt>
+                <c:pt idx="344">
+                  <c:v>45170</c:v>
+                </c:pt>
+                <c:pt idx="345">
+                  <c:v>45200</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -2328,6 +2337,12 @@
                 </c:pt>
                 <c:pt idx="343">
                   <c:v>8.8703735811575105E-2</c:v>
+                </c:pt>
+                <c:pt idx="344">
+                  <c:v>8.69610556503468E-2</c:v>
+                </c:pt>
+                <c:pt idx="345">
+                  <c:v>8.5154952330852907E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3411,8 +3426,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:RX349"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A313" workbookViewId="0">
-      <selection activeCell="D346" sqref="D346"/>
+    <sheetView tabSelected="1" topLeftCell="A317" workbookViewId="0">
+      <selection activeCell="B347" sqref="B347"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3429,10 +3444,10 @@
       </c>
     </row>
     <row r="2" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="9" t="s">
         <v>1</v>
       </c>
       <c r="CG2" s="1"/>
@@ -3468,10 +3483,10 @@
       <c r="RX2" s="1"/>
     </row>
     <row r="3" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
+      <c r="A3" s="7">
         <v>34700</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="8">
         <v>3.5906071097335332E-2</v>
       </c>
       <c r="CG3" s="1"/>
@@ -3505,10 +3520,10 @@
       <c r="RX3" s="1"/>
     </row>
     <row r="4" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
+      <c r="A4" s="7">
         <v>34731</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="8">
         <v>4.641371511935781E-2</v>
       </c>
       <c r="CG4" s="1"/>
@@ -3542,10 +3557,10 @@
       <c r="RX4" s="1"/>
     </row>
     <row r="5" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
+      <c r="A5" s="7">
         <v>34759</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="8">
         <v>6.8188691890601116E-2</v>
       </c>
       <c r="CG5" s="1"/>
@@ -3578,10 +3593,10 @@
       <c r="RX5" s="1"/>
     </row>
     <row r="6" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
+      <c r="A6" s="7">
         <v>34790</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="8">
         <v>9.0011601145643869E-2</v>
       </c>
       <c r="CG6" s="1"/>
@@ -3612,10 +3627,10 @@
       <c r="RM6" s="1"/>
     </row>
     <row r="7" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
+      <c r="A7" s="7">
         <v>34820</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="8">
         <v>9.9496073670305801E-2</v>
       </c>
       <c r="CG7" s="1"/>
@@ -3645,10 +3660,10 @@
       <c r="RM7" s="1"/>
     </row>
     <row r="8" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
+      <c r="A8" s="7">
         <v>34851</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="8">
         <v>0.11863771466397069</v>
       </c>
       <c r="CG8" s="1"/>
@@ -3678,10 +3693,10 @@
       <c r="RM8" s="1"/>
     </row>
     <row r="9" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
+      <c r="A9" s="7">
         <v>34881</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="8">
         <v>0.1181146572660678</v>
       </c>
       <c r="CG9" s="1"/>
@@ -3701,10 +3716,10 @@
       <c r="RM9" s="1"/>
     </row>
     <row r="10" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
+      <c r="A10" s="7">
         <v>34912</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="8">
         <v>0.11925440378813899</v>
       </c>
       <c r="CG10" s="1"/>
@@ -3723,10 +3738,10 @@
       <c r="RM10" s="1"/>
     </row>
     <row r="11" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
+      <c r="A11" s="7">
         <v>34943</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="8">
         <v>8.0427229515112636E-2</v>
       </c>
       <c r="CG11" s="1"/>
@@ -3745,10 +3760,10 @@
       <c r="RM11" s="1"/>
     </row>
     <row r="12" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A12" s="5">
+      <c r="A12" s="7">
         <v>34973</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="8">
         <v>9.2888414728135582E-2</v>
       </c>
       <c r="CG12" s="1"/>
@@ -3766,10 +3781,10 @@
       <c r="RM12" s="1"/>
     </row>
     <row r="13" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A13" s="5">
+      <c r="A13" s="7">
         <v>35004</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="8">
         <v>0.10118496200041718</v>
       </c>
       <c r="CG13" s="1"/>
@@ -3787,10 +3802,10 @@
       <c r="RM13" s="1"/>
     </row>
     <row r="14" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
+      <c r="A14" s="7">
         <v>35034</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="8">
         <v>0.10732542683580969</v>
       </c>
       <c r="CG14" s="1"/>
@@ -3806,10 +3821,10 @@
       <c r="OY14" s="1"/>
     </row>
     <row r="15" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A15" s="5">
+      <c r="A15" s="7">
         <v>35065</v>
       </c>
-      <c r="B15" s="6">
+      <c r="B15" s="8">
         <v>9.1621260099534085E-2</v>
       </c>
       <c r="CG15" s="1"/>
@@ -3825,665 +3840,665 @@
       <c r="OY15" s="1"/>
     </row>
     <row r="16" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A16" s="5">
+      <c r="A16" s="7">
         <v>35096</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B16" s="8">
         <v>8.4905503970074639E-2</v>
       </c>
       <c r="CP16" s="1"/>
     </row>
     <row r="17" spans="1:94" x14ac:dyDescent="0.25">
-      <c r="A17" s="5">
+      <c r="A17" s="7">
         <v>35125</v>
       </c>
-      <c r="B17" s="6">
+      <c r="B17" s="8">
         <v>0.10049276040389069</v>
       </c>
       <c r="CP17" s="1"/>
     </row>
     <row r="18" spans="1:94" x14ac:dyDescent="0.25">
-      <c r="A18" s="5">
+      <c r="A18" s="7">
         <v>35156</v>
       </c>
-      <c r="B18" s="6">
+      <c r="B18" s="8">
         <v>9.6531384813158941E-2</v>
       </c>
       <c r="CP18" s="1"/>
     </row>
     <row r="19" spans="1:94" x14ac:dyDescent="0.25">
-      <c r="A19" s="5">
+      <c r="A19" s="7">
         <v>35186</v>
       </c>
-      <c r="B19" s="6">
+      <c r="B19" s="8">
         <v>9.5088188666882692E-2</v>
       </c>
       <c r="CP19" s="1"/>
     </row>
     <row r="20" spans="1:94" x14ac:dyDescent="0.25">
-      <c r="A20" s="5">
+      <c r="A20" s="7">
         <v>35217</v>
       </c>
-      <c r="B20" s="6">
+      <c r="B20" s="8">
         <v>9.0796583575804307E-2</v>
       </c>
       <c r="CP20" s="1"/>
     </row>
     <row r="21" spans="1:94" x14ac:dyDescent="0.25">
-      <c r="A21" s="5">
+      <c r="A21" s="7">
         <v>35247</v>
       </c>
-      <c r="B21" s="6">
+      <c r="B21" s="8">
         <v>9.2623876599203819E-2</v>
       </c>
       <c r="CP21" s="1"/>
     </row>
     <row r="22" spans="1:94" x14ac:dyDescent="0.25">
-      <c r="A22" s="5">
+      <c r="A22" s="7">
         <v>35278</v>
       </c>
-      <c r="B22" s="6">
+      <c r="B22" s="8">
         <v>9.1099901245860898E-2</v>
       </c>
       <c r="CP22" s="1"/>
     </row>
     <row r="23" spans="1:94" x14ac:dyDescent="0.25">
-      <c r="A23" s="5">
+      <c r="A23" s="7">
         <v>35309</v>
       </c>
-      <c r="B23" s="6">
+      <c r="B23" s="8">
         <v>9.2854806609296375E-2</v>
       </c>
       <c r="CP23" s="1"/>
     </row>
     <row r="24" spans="1:94" x14ac:dyDescent="0.25">
-      <c r="A24" s="5">
+      <c r="A24" s="7">
         <v>35339</v>
       </c>
-      <c r="B24" s="6">
+      <c r="B24" s="8">
         <v>0.10127373741409153</v>
       </c>
       <c r="CP24" s="1"/>
     </row>
     <row r="25" spans="1:94" x14ac:dyDescent="0.25">
-      <c r="A25" s="5">
+      <c r="A25" s="7">
         <v>35370</v>
       </c>
-      <c r="B25" s="6">
+      <c r="B25" s="8">
         <v>0.10142804442282341</v>
       </c>
       <c r="CP25" s="1"/>
     </row>
     <row r="26" spans="1:94" x14ac:dyDescent="0.25">
-      <c r="A26" s="5">
+      <c r="A26" s="7">
         <v>35400</v>
       </c>
-      <c r="B26" s="6">
+      <c r="B26" s="8">
         <v>9.9700000278104189E-2</v>
       </c>
       <c r="CP26" s="1"/>
     </row>
     <row r="27" spans="1:94" x14ac:dyDescent="0.25">
-      <c r="A27" s="5">
+      <c r="A27" s="7">
         <v>35431</v>
       </c>
-      <c r="B27" s="6">
+      <c r="B27" s="8">
         <v>9.7052332691215076E-2</v>
       </c>
       <c r="CP27" s="1"/>
     </row>
     <row r="28" spans="1:94" x14ac:dyDescent="0.25">
-      <c r="A28" s="5">
+      <c r="A28" s="7">
         <v>35462</v>
       </c>
-      <c r="B28" s="6">
+      <c r="B28" s="8">
         <v>9.1057142830797522E-2</v>
       </c>
       <c r="CP28" s="1"/>
     </row>
     <row r="29" spans="1:94" x14ac:dyDescent="0.25">
-      <c r="A29" s="5">
+      <c r="A29" s="7">
         <v>35490</v>
       </c>
-      <c r="B29" s="6">
+      <c r="B29" s="8">
         <v>8.6177248797735806E-2</v>
       </c>
       <c r="CP29" s="1"/>
     </row>
     <row r="30" spans="1:94" x14ac:dyDescent="0.25">
-      <c r="A30" s="5">
+      <c r="A30" s="7">
         <v>35521</v>
       </c>
-      <c r="B30" s="6">
+      <c r="B30" s="8">
         <v>8.5066948095953776E-2</v>
       </c>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="4"/>
-      <c r="I30" s="4"/>
-      <c r="J30" s="4"/>
-      <c r="K30" s="4"/>
-      <c r="L30" s="4"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="6"/>
+      <c r="K30" s="6"/>
+      <c r="L30" s="6"/>
       <c r="CP30" s="1"/>
     </row>
     <row r="31" spans="1:94" x14ac:dyDescent="0.25">
-      <c r="A31" s="5">
+      <c r="A31" s="7">
         <v>35551</v>
       </c>
-      <c r="B31" s="6">
+      <c r="B31" s="8">
         <v>9.7288837160340563E-2</v>
       </c>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
-      <c r="H31" s="4"/>
-      <c r="I31" s="4"/>
-      <c r="J31" s="4"/>
-      <c r="K31" s="4"/>
-      <c r="L31" s="4"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="6"/>
+      <c r="K31" s="6"/>
+      <c r="L31" s="6"/>
       <c r="CP31" s="1"/>
     </row>
     <row r="32" spans="1:94" x14ac:dyDescent="0.25">
-      <c r="A32" s="5">
+      <c r="A32" s="7">
         <v>35582</v>
       </c>
-      <c r="B32" s="6">
+      <c r="B32" s="8">
         <v>9.6957468174919514E-2</v>
       </c>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
-      <c r="H32" s="4"/>
-      <c r="I32" s="4"/>
-      <c r="J32" s="4"/>
-      <c r="K32" s="4"/>
-      <c r="L32" s="4"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
+      <c r="I32" s="6"/>
+      <c r="J32" s="6"/>
+      <c r="K32" s="6"/>
+      <c r="L32" s="6"/>
       <c r="CP32" s="1"/>
     </row>
     <row r="33" spans="1:94" x14ac:dyDescent="0.25">
-      <c r="A33" s="5">
+      <c r="A33" s="7">
         <v>35612</v>
       </c>
-      <c r="B33" s="6">
+      <c r="B33" s="8">
         <v>9.8258192485687817E-2</v>
       </c>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
-      <c r="H33" s="4"/>
-      <c r="I33" s="4"/>
-      <c r="J33" s="4"/>
-      <c r="K33" s="4"/>
-      <c r="L33" s="4"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="6"/>
+      <c r="J33" s="6"/>
+      <c r="K33" s="6"/>
+      <c r="L33" s="6"/>
       <c r="CP33" s="1"/>
     </row>
     <row r="34" spans="1:94" x14ac:dyDescent="0.25">
-      <c r="A34" s="5">
+      <c r="A34" s="7">
         <v>35643</v>
       </c>
-      <c r="B34" s="6">
+      <c r="B34" s="8">
         <v>0.10071108991221206</v>
       </c>
-      <c r="L34" s="4"/>
+      <c r="L34" s="6"/>
       <c r="CP34" s="1"/>
     </row>
     <row r="35" spans="1:94" x14ac:dyDescent="0.25">
-      <c r="A35" s="5">
+      <c r="A35" s="7">
         <v>35674</v>
       </c>
-      <c r="B35" s="6">
+      <c r="B35" s="8">
         <v>9.4101292650451321E-2</v>
       </c>
       <c r="CP35" s="1"/>
     </row>
     <row r="36" spans="1:94" x14ac:dyDescent="0.25">
-      <c r="A36" s="5">
+      <c r="A36" s="7">
         <v>35704</v>
       </c>
-      <c r="B36" s="6">
+      <c r="B36" s="8">
         <v>0.1022443853346008</v>
       </c>
       <c r="CP36" s="1"/>
     </row>
     <row r="37" spans="1:94" x14ac:dyDescent="0.25">
-      <c r="A37" s="5">
+      <c r="A37" s="7">
         <v>35735</v>
       </c>
-      <c r="B37" s="6">
+      <c r="B37" s="8">
         <v>0.11673503599412813</v>
       </c>
       <c r="CP37" s="1"/>
     </row>
     <row r="38" spans="1:94" x14ac:dyDescent="0.25">
-      <c r="A38" s="5">
+      <c r="A38" s="7">
         <v>35765</v>
       </c>
-      <c r="B38" s="6">
+      <c r="B38" s="8">
         <v>0.12868892588777975</v>
       </c>
       <c r="CP38" s="1"/>
     </row>
     <row r="39" spans="1:94" x14ac:dyDescent="0.25">
-      <c r="A39" s="5">
+      <c r="A39" s="7">
         <v>35796</v>
       </c>
-      <c r="B39" s="6">
+      <c r="B39" s="8">
         <v>0.13246738378006745</v>
       </c>
       <c r="CP39" s="1"/>
     </row>
     <row r="40" spans="1:94" x14ac:dyDescent="0.25">
-      <c r="A40" s="5">
+      <c r="A40" s="7">
         <v>35827</v>
       </c>
-      <c r="B40" s="6">
+      <c r="B40" s="8">
         <v>0.12192540989307418</v>
       </c>
       <c r="CP40" s="1"/>
     </row>
     <row r="41" spans="1:94" x14ac:dyDescent="0.25">
-      <c r="A41" s="5">
+      <c r="A41" s="7">
         <v>35855</v>
       </c>
-      <c r="B41" s="6">
+      <c r="B41" s="8">
         <v>0.11858185629167939</v>
       </c>
       <c r="CP41" s="1"/>
     </row>
     <row r="42" spans="1:94" x14ac:dyDescent="0.25">
-      <c r="A42" s="5">
+      <c r="A42" s="7">
         <v>35886</v>
       </c>
-      <c r="B42" s="6">
+      <c r="B42" s="8">
         <v>0.11009539820274278</v>
       </c>
       <c r="CP42" s="1"/>
     </row>
     <row r="43" spans="1:94" x14ac:dyDescent="0.25">
-      <c r="A43" s="5">
+      <c r="A43" s="7">
         <v>35916</v>
       </c>
-      <c r="B43" s="6">
+      <c r="B43" s="8">
         <v>0.14815671762109539</v>
       </c>
       <c r="CP43" s="1"/>
     </row>
     <row r="44" spans="1:94" x14ac:dyDescent="0.25">
-      <c r="A44" s="5">
+      <c r="A44" s="7">
         <v>35947</v>
       </c>
-      <c r="B44" s="6">
+      <c r="B44" s="8">
         <v>0.16414072309545738</v>
       </c>
       <c r="CP44" s="1"/>
     </row>
     <row r="45" spans="1:94" x14ac:dyDescent="0.25">
-      <c r="A45" s="5">
+      <c r="A45" s="7">
         <v>35977</v>
       </c>
-      <c r="B45" s="6">
+      <c r="B45" s="8">
         <v>0.15684487547919845</v>
       </c>
       <c r="CP45" s="1"/>
     </row>
     <row r="46" spans="1:94" x14ac:dyDescent="0.25">
-      <c r="A46" s="5">
+      <c r="A46" s="7">
         <v>36008</v>
       </c>
-      <c r="B46" s="6">
+      <c r="B46" s="8">
         <v>0.20761986410571115</v>
       </c>
       <c r="CP46" s="1"/>
     </row>
     <row r="47" spans="1:94" x14ac:dyDescent="0.25">
-      <c r="A47" s="5">
+      <c r="A47" s="7">
         <v>36039</v>
       </c>
-      <c r="B47" s="6">
+      <c r="B47" s="8">
         <v>0.26488372425157419</v>
       </c>
       <c r="CP47" s="1"/>
     </row>
     <row r="48" spans="1:94" x14ac:dyDescent="0.25">
-      <c r="A48" s="5">
+      <c r="A48" s="7">
         <v>36069</v>
       </c>
-      <c r="B48" s="6">
+      <c r="B48" s="8">
         <v>0.27386908893169182</v>
       </c>
       <c r="CP48" s="1"/>
     </row>
     <row r="49" spans="1:94" x14ac:dyDescent="0.25">
-      <c r="A49" s="5">
+      <c r="A49" s="7">
         <v>36100</v>
       </c>
-      <c r="B49" s="6">
+      <c r="B49" s="8">
         <v>0.23368482800820384</v>
       </c>
       <c r="CP49" s="1"/>
     </row>
     <row r="50" spans="1:94" x14ac:dyDescent="0.25">
-      <c r="A50" s="5">
+      <c r="A50" s="7">
         <v>36130</v>
       </c>
-      <c r="B50" s="6">
+      <c r="B50" s="8">
         <v>0.19728157436806892</v>
       </c>
       <c r="CP50" s="1"/>
     </row>
     <row r="51" spans="1:94" x14ac:dyDescent="0.25">
-      <c r="A51" s="5">
+      <c r="A51" s="7">
         <v>36161</v>
       </c>
-      <c r="B51" s="6">
+      <c r="B51" s="8">
         <v>0.18849719620951449</v>
       </c>
-      <c r="D51" s="2"/>
+      <c r="D51" s="4"/>
       <c r="CP51" s="1"/>
     </row>
     <row r="52" spans="1:94" x14ac:dyDescent="0.25">
-      <c r="A52" s="5">
+      <c r="A52" s="7">
         <v>36192</v>
       </c>
-      <c r="B52" s="6">
+      <c r="B52" s="8">
         <v>0.17879547863724937</v>
       </c>
-      <c r="D52" s="2"/>
+      <c r="D52" s="4"/>
       <c r="CP52" s="1"/>
     </row>
     <row r="53" spans="1:94" x14ac:dyDescent="0.25">
-      <c r="A53" s="5">
+      <c r="A53" s="7">
         <v>36220</v>
       </c>
-      <c r="B53" s="6">
+      <c r="B53" s="8">
         <v>0.19521218246374467</v>
       </c>
-      <c r="D53" s="2"/>
+      <c r="D53" s="4"/>
       <c r="CP53" s="1"/>
     </row>
     <row r="54" spans="1:94" x14ac:dyDescent="0.25">
-      <c r="A54" s="5">
+      <c r="A54" s="7">
         <v>36251</v>
       </c>
-      <c r="B54" s="6">
+      <c r="B54" s="8">
         <v>0.17667737273699313</v>
       </c>
-      <c r="D54" s="2"/>
+      <c r="D54" s="4"/>
       <c r="CP54" s="1"/>
     </row>
     <row r="55" spans="1:94" x14ac:dyDescent="0.25">
-      <c r="A55" s="5">
+      <c r="A55" s="7">
         <v>36281</v>
       </c>
-      <c r="B55" s="6">
+      <c r="B55" s="8">
         <v>0.17240854293261376</v>
       </c>
-      <c r="D55" s="2"/>
+      <c r="D55" s="4"/>
       <c r="CP55" s="1"/>
     </row>
     <row r="56" spans="1:94" x14ac:dyDescent="0.25">
-      <c r="A56" s="5">
+      <c r="A56" s="7">
         <v>36312</v>
       </c>
-      <c r="B56" s="6">
+      <c r="B56" s="8">
         <v>0.15905547118167043</v>
       </c>
-      <c r="D56" s="2"/>
+      <c r="D56" s="4"/>
       <c r="CP56" s="1"/>
     </row>
     <row r="57" spans="1:94" x14ac:dyDescent="0.25">
-      <c r="A57" s="5">
+      <c r="A57" s="7">
         <v>36342</v>
       </c>
-      <c r="B57" s="6">
+      <c r="B57" s="8">
         <v>0.15865389804394955</v>
       </c>
-      <c r="D57" s="2"/>
+      <c r="D57" s="4"/>
       <c r="CP57" s="1"/>
     </row>
     <row r="58" spans="1:94" x14ac:dyDescent="0.25">
-      <c r="A58" s="5">
+      <c r="A58" s="7">
         <v>36373</v>
       </c>
-      <c r="B58" s="6">
+      <c r="B58" s="8">
         <v>0.15275419272689961</v>
       </c>
-      <c r="D58" s="2"/>
+      <c r="D58" s="4"/>
       <c r="CP58" s="1"/>
     </row>
     <row r="59" spans="1:94" x14ac:dyDescent="0.25">
-      <c r="A59" s="5">
+      <c r="A59" s="7">
         <v>36404</v>
       </c>
-      <c r="B59" s="6">
+      <c r="B59" s="8">
         <v>0.13159865421370617</v>
       </c>
-      <c r="D59" s="2"/>
+      <c r="D59" s="4"/>
       <c r="CP59" s="1"/>
     </row>
     <row r="60" spans="1:94" x14ac:dyDescent="0.25">
-      <c r="A60" s="5">
+      <c r="A60" s="7">
         <v>36434</v>
       </c>
-      <c r="B60" s="6">
+      <c r="B60" s="8">
         <v>0.12196728595845485</v>
       </c>
-      <c r="D60" s="2"/>
+      <c r="D60" s="4"/>
       <c r="CP60" s="1"/>
     </row>
     <row r="61" spans="1:94" x14ac:dyDescent="0.25">
-      <c r="A61" s="5">
+      <c r="A61" s="7">
         <v>36465</v>
       </c>
-      <c r="B61" s="6">
+      <c r="B61" s="8">
         <v>0.10437517943413213</v>
       </c>
-      <c r="D61" s="2"/>
+      <c r="D61" s="4"/>
       <c r="CP61" s="1"/>
     </row>
     <row r="62" spans="1:94" x14ac:dyDescent="0.25">
-      <c r="A62" s="5">
+      <c r="A62" s="7">
         <v>36495</v>
       </c>
-      <c r="B62" s="6">
+      <c r="B62" s="8">
         <v>8.4895285767080067E-2</v>
       </c>
-      <c r="D62" s="2"/>
+      <c r="D62" s="4"/>
       <c r="CP62" s="1"/>
     </row>
     <row r="63" spans="1:94" x14ac:dyDescent="0.25">
-      <c r="A63" s="5">
+      <c r="A63" s="7">
         <v>36526</v>
       </c>
-      <c r="B63" s="6">
+      <c r="B63" s="8">
         <v>8.0964220165040707E-2</v>
       </c>
-      <c r="D63" s="2"/>
+      <c r="D63" s="4"/>
       <c r="CP63" s="1"/>
     </row>
     <row r="64" spans="1:94" x14ac:dyDescent="0.25">
-      <c r="A64" s="5">
+      <c r="A64" s="7">
         <v>36557</v>
       </c>
-      <c r="B64" s="6">
+      <c r="B64" s="8">
         <v>8.5143819747368649E-2</v>
       </c>
-      <c r="D64" s="2"/>
+      <c r="D64" s="4"/>
       <c r="CP64" s="1"/>
     </row>
     <row r="65" spans="1:94" x14ac:dyDescent="0.25">
-      <c r="A65" s="5">
+      <c r="A65" s="7">
         <v>36586</v>
       </c>
-      <c r="B65" s="6">
+      <c r="B65" s="8">
         <v>9.4432793059799777E-2</v>
       </c>
-      <c r="D65" s="2"/>
-      <c r="E65" s="2"/>
+      <c r="D65" s="4"/>
+      <c r="E65" s="4"/>
       <c r="CP65" s="1"/>
     </row>
     <row r="66" spans="1:94" x14ac:dyDescent="0.25">
-      <c r="A66" s="5">
+      <c r="A66" s="7">
         <v>36617</v>
       </c>
-      <c r="B66" s="6">
+      <c r="B66" s="8">
         <v>0.1068984082862578</v>
       </c>
-      <c r="D66" s="2"/>
-      <c r="E66" s="2"/>
+      <c r="D66" s="4"/>
+      <c r="E66" s="4"/>
       <c r="CP66" s="1"/>
     </row>
     <row r="67" spans="1:94" x14ac:dyDescent="0.25">
-      <c r="A67" s="5">
+      <c r="A67" s="7">
         <v>36647</v>
       </c>
-      <c r="B67" s="6">
+      <c r="B67" s="8">
         <v>0.10194024162250852</v>
       </c>
-      <c r="D67" s="2"/>
-      <c r="E67" s="2"/>
+      <c r="D67" s="4"/>
+      <c r="E67" s="4"/>
       <c r="CP67" s="1"/>
     </row>
     <row r="68" spans="1:94" x14ac:dyDescent="0.25">
-      <c r="A68" s="5">
+      <c r="A68" s="7">
         <v>36678</v>
       </c>
-      <c r="B68" s="6">
+      <c r="B68" s="8">
         <v>0.11520688931942046</v>
       </c>
-      <c r="D68" s="2"/>
-      <c r="E68" s="2"/>
+      <c r="D68" s="4"/>
+      <c r="E68" s="4"/>
       <c r="CP68" s="1"/>
     </row>
     <row r="69" spans="1:94" x14ac:dyDescent="0.25">
-      <c r="A69" s="5">
+      <c r="A69" s="7">
         <v>36708</v>
       </c>
-      <c r="B69" s="6">
+      <c r="B69" s="8">
         <v>0.10847862629401375</v>
       </c>
-      <c r="E69" s="2"/>
+      <c r="E69" s="4"/>
       <c r="CP69" s="1"/>
     </row>
     <row r="70" spans="1:94" x14ac:dyDescent="0.25">
-      <c r="A70" s="5">
+      <c r="A70" s="7">
         <v>36739</v>
       </c>
-      <c r="B70" s="6">
+      <c r="B70" s="8">
         <v>0.11669317806908461</v>
       </c>
-      <c r="E70" s="2"/>
+      <c r="E70" s="4"/>
       <c r="CP70" s="1"/>
     </row>
     <row r="71" spans="1:94" x14ac:dyDescent="0.25">
-      <c r="A71" s="5">
+      <c r="A71" s="7">
         <v>36770</v>
       </c>
-      <c r="B71" s="6">
+      <c r="B71" s="8">
         <v>0.12461879502315275</v>
       </c>
-      <c r="E71" s="2"/>
+      <c r="E71" s="4"/>
       <c r="CP71" s="1"/>
     </row>
     <row r="72" spans="1:94" x14ac:dyDescent="0.25">
-      <c r="A72" s="5">
+      <c r="A72" s="7">
         <v>36800</v>
       </c>
-      <c r="B72" s="6">
+      <c r="B72" s="8">
         <v>0.12350351608453644</v>
       </c>
-      <c r="E72" s="2"/>
+      <c r="E72" s="4"/>
       <c r="CP72" s="1"/>
     </row>
     <row r="73" spans="1:94" x14ac:dyDescent="0.25">
-      <c r="A73" s="5">
+      <c r="A73" s="7">
         <v>36831</v>
       </c>
-      <c r="B73" s="6">
+      <c r="B73" s="8">
         <v>0.13624280260074831</v>
       </c>
-      <c r="E73" s="2"/>
+      <c r="E73" s="4"/>
       <c r="CP73" s="1"/>
     </row>
     <row r="74" spans="1:94" x14ac:dyDescent="0.25">
-      <c r="A74" s="5">
+      <c r="A74" s="7">
         <v>36861</v>
       </c>
-      <c r="B74" s="6">
+      <c r="B74" s="8">
         <v>0.10449451374749155</v>
       </c>
-      <c r="E74" s="2"/>
+      <c r="E74" s="4"/>
       <c r="CP74" s="1"/>
     </row>
     <row r="75" spans="1:94" x14ac:dyDescent="0.25">
-      <c r="A75" s="5">
+      <c r="A75" s="7">
         <v>36892</v>
       </c>
-      <c r="B75" s="6">
+      <c r="B75" s="8">
         <v>9.8078739800215115E-2</v>
       </c>
-      <c r="E75" s="2"/>
+      <c r="E75" s="4"/>
       <c r="CP75" s="1"/>
     </row>
     <row r="76" spans="1:94" x14ac:dyDescent="0.25">
-      <c r="A76" s="5">
+      <c r="A76" s="7">
         <v>36923</v>
       </c>
-      <c r="B76" s="6">
+      <c r="B76" s="8">
         <v>9.4986612102584869E-2</v>
       </c>
-      <c r="E76" s="2"/>
+      <c r="E76" s="4"/>
       <c r="CP76" s="1"/>
     </row>
     <row r="77" spans="1:94" x14ac:dyDescent="0.25">
-      <c r="A77" s="5">
+      <c r="A77" s="7">
         <v>36951</v>
       </c>
-      <c r="B77" s="6">
+      <c r="B77" s="8">
         <v>0.10943199261845223</v>
       </c>
-      <c r="E77" s="2"/>
+      <c r="E77" s="4"/>
       <c r="CP77" s="1"/>
     </row>
     <row r="78" spans="1:94" x14ac:dyDescent="0.25">
-      <c r="A78" s="5">
+      <c r="A78" s="7">
         <v>36982</v>
       </c>
-      <c r="B78" s="6">
+      <c r="B78" s="8">
         <v>0.10230821441197835</v>
       </c>
-      <c r="E78" s="2"/>
+      <c r="E78" s="4"/>
       <c r="CP78" s="1"/>
     </row>
     <row r="79" spans="1:94" x14ac:dyDescent="0.25">
-      <c r="A79" s="5">
+      <c r="A79" s="7">
         <v>37012</v>
       </c>
-      <c r="B79" s="6">
+      <c r="B79" s="8">
         <v>0.11448510925596571</v>
       </c>
-      <c r="E79" s="2"/>
+      <c r="E79" s="4"/>
       <c r="CP79" s="1"/>
     </row>
     <row r="80" spans="1:94" x14ac:dyDescent="0.25">
-      <c r="A80" s="5">
+      <c r="A80" s="7">
         <v>37043</v>
       </c>
-      <c r="B80" s="6">
+      <c r="B80" s="8">
         <v>0.12205193419326613</v>
       </c>
-      <c r="E80" s="2"/>
+      <c r="E80" s="4"/>
       <c r="CP80" s="1"/>
     </row>
     <row r="81" spans="1:206" x14ac:dyDescent="0.25">
-      <c r="A81" s="5">
+      <c r="A81" s="7">
         <v>37073</v>
       </c>
-      <c r="B81" s="6">
+      <c r="B81" s="8">
         <v>0.12472087316217893</v>
       </c>
-      <c r="E81" s="2"/>
+      <c r="E81" s="4"/>
       <c r="CP81" s="1"/>
       <c r="DC81" s="1"/>
       <c r="DE81" s="1"/>
@@ -4495,10 +4510,10 @@
       <c r="DK81" s="1"/>
     </row>
     <row r="82" spans="1:206" x14ac:dyDescent="0.25">
-      <c r="A82" s="5">
+      <c r="A82" s="7">
         <v>37104</v>
       </c>
-      <c r="B82" s="6">
+      <c r="B82" s="8">
         <v>0.13164962330151575</v>
       </c>
       <c r="CP82" s="1"/>
@@ -4512,10 +4527,10 @@
       <c r="DK82" s="1"/>
     </row>
     <row r="83" spans="1:206" x14ac:dyDescent="0.25">
-      <c r="A83" s="5">
+      <c r="A83" s="7">
         <v>37135</v>
       </c>
-      <c r="B83" s="6">
+      <c r="B83" s="8">
         <v>0.16920274455915726</v>
       </c>
       <c r="CP83" s="1"/>
@@ -4530,10 +4545,10 @@
       <c r="FQ83" s="1"/>
     </row>
     <row r="84" spans="1:206" x14ac:dyDescent="0.25">
-      <c r="A84" s="5">
+      <c r="A84" s="7">
         <v>37165</v>
       </c>
-      <c r="B84" s="6">
+      <c r="B84" s="8">
         <v>0.16487384010580458</v>
       </c>
       <c r="CP84" s="1"/>
@@ -4548,10 +4563,10 @@
       <c r="FQ84" s="1"/>
     </row>
     <row r="85" spans="1:206" x14ac:dyDescent="0.25">
-      <c r="A85" s="5">
+      <c r="A85" s="7">
         <v>37196</v>
       </c>
-      <c r="B85" s="6">
+      <c r="B85" s="8">
         <v>0.14485365882340293</v>
       </c>
       <c r="CP85" s="1"/>
@@ -4566,10 +4581,10 @@
       <c r="FQ85" s="1"/>
     </row>
     <row r="86" spans="1:206" x14ac:dyDescent="0.25">
-      <c r="A86" s="5">
+      <c r="A86" s="7">
         <v>37226</v>
       </c>
-      <c r="B86" s="6">
+      <c r="B86" s="8">
         <v>0.12057147500114479</v>
       </c>
       <c r="CP86" s="1"/>
@@ -4584,10 +4599,10 @@
       <c r="FQ86" s="1"/>
     </row>
     <row r="87" spans="1:206" x14ac:dyDescent="0.25">
-      <c r="A87" s="5">
+      <c r="A87" s="7">
         <v>37257</v>
       </c>
-      <c r="B87" s="6">
+      <c r="B87" s="8">
         <v>0.12028644057053653</v>
       </c>
       <c r="CP87" s="1"/>
@@ -4602,10 +4617,10 @@
       <c r="FQ87" s="1"/>
     </row>
     <row r="88" spans="1:206" x14ac:dyDescent="0.25">
-      <c r="A88" s="5">
+      <c r="A88" s="7">
         <v>37288</v>
       </c>
-      <c r="B88" s="6">
+      <c r="B88" s="8">
         <v>0.11585635189852062</v>
       </c>
       <c r="CP88" s="1"/>
@@ -4620,10 +4635,10 @@
       <c r="FQ88" s="1"/>
     </row>
     <row r="89" spans="1:206" x14ac:dyDescent="0.25">
-      <c r="A89" s="5">
+      <c r="A89" s="7">
         <v>37316</v>
       </c>
-      <c r="B89" s="6">
+      <c r="B89" s="8">
         <v>0.12274527752297042</v>
       </c>
       <c r="CP89" s="1"/>
@@ -4639,10 +4654,10 @@
       <c r="FQ89" s="1"/>
     </row>
     <row r="90" spans="1:206" x14ac:dyDescent="0.25">
-      <c r="A90" s="5">
+      <c r="A90" s="7">
         <v>37347</v>
       </c>
-      <c r="B90" s="6">
+      <c r="B90" s="8">
         <v>0.12101568147782529</v>
       </c>
       <c r="CP90" s="1"/>
@@ -4658,10 +4673,10 @@
       <c r="FQ90" s="1"/>
     </row>
     <row r="91" spans="1:206" x14ac:dyDescent="0.25">
-      <c r="A91" s="5">
+      <c r="A91" s="7">
         <v>37377</v>
       </c>
-      <c r="B91" s="6">
+      <c r="B91" s="8">
         <v>0.13834911739732181</v>
       </c>
       <c r="CP91" s="1"/>
@@ -4677,10 +4692,10 @@
       <c r="FQ91" s="1"/>
     </row>
     <row r="92" spans="1:206" x14ac:dyDescent="0.25">
-      <c r="A92" s="5">
+      <c r="A92" s="7">
         <v>37408</v>
       </c>
-      <c r="B92" s="6">
+      <c r="B92" s="8">
         <v>0.13898444661446926</v>
       </c>
       <c r="CP92" s="1"/>
@@ -4697,10 +4712,10 @@
       <c r="FQ92" s="1"/>
     </row>
     <row r="93" spans="1:206" x14ac:dyDescent="0.25">
-      <c r="A93" s="5">
+      <c r="A93" s="7">
         <v>37438</v>
       </c>
-      <c r="B93" s="6">
+      <c r="B93" s="8">
         <v>0.15154676452080135</v>
       </c>
       <c r="CP93" s="1"/>
@@ -4717,10 +4732,10 @@
       <c r="FQ93" s="1"/>
     </row>
     <row r="94" spans="1:206" x14ac:dyDescent="0.25">
-      <c r="A94" s="5">
+      <c r="A94" s="7">
         <v>37469</v>
       </c>
-      <c r="B94" s="6">
+      <c r="B94" s="8">
         <v>0.14914501917668246</v>
       </c>
       <c r="CP94" s="1"/>
@@ -4737,10 +4752,10 @@
       <c r="FQ94" s="1"/>
     </row>
     <row r="95" spans="1:206" x14ac:dyDescent="0.25">
-      <c r="A95" s="5">
+      <c r="A95" s="7">
         <v>37500</v>
       </c>
-      <c r="B95" s="6">
+      <c r="B95" s="8">
         <v>0.17729158577688089</v>
       </c>
       <c r="CP95" s="1"/>
@@ -4758,10 +4773,10 @@
       <c r="GX95" s="1"/>
     </row>
     <row r="96" spans="1:206" x14ac:dyDescent="0.25">
-      <c r="A96" s="5">
+      <c r="A96" s="7">
         <v>37530</v>
       </c>
-      <c r="B96" s="6">
+      <c r="B96" s="8">
         <v>0.16158417270187989</v>
       </c>
       <c r="CP96" s="1"/>
@@ -4779,10 +4794,10 @@
       <c r="GX96" s="1"/>
     </row>
     <row r="97" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A97" s="5">
+      <c r="A97" s="7">
         <v>37561</v>
       </c>
-      <c r="B97" s="6">
+      <c r="B97" s="8">
         <v>0.15765516285709646</v>
       </c>
       <c r="CG97" s="1"/>
@@ -4810,10 +4825,10 @@
       <c r="QQ97" s="1"/>
     </row>
     <row r="98" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A98" s="5">
+      <c r="A98" s="7">
         <v>37591</v>
       </c>
-      <c r="B98" s="6">
+      <c r="B98" s="8">
         <v>0.16155516390609645</v>
       </c>
       <c r="CG98" s="1"/>
@@ -4841,10 +4856,10 @@
       <c r="QQ98" s="1"/>
     </row>
     <row r="99" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A99" s="5">
+      <c r="A99" s="7">
         <v>37622</v>
       </c>
-      <c r="B99" s="6">
+      <c r="B99" s="8">
         <v>0.16721818984210535</v>
       </c>
       <c r="CG99" s="1"/>
@@ -4881,10 +4896,10 @@
       <c r="QQ99" s="1"/>
     </row>
     <row r="100" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A100" s="5">
+      <c r="A100" s="7">
         <v>37653</v>
       </c>
-      <c r="B100" s="6">
+      <c r="B100" s="8">
         <v>0.16873740603929704</v>
       </c>
       <c r="CG100" s="1"/>
@@ -4931,10 +4946,10 @@
       <c r="QQ100" s="1"/>
     </row>
     <row r="101" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A101" s="5">
+      <c r="A101" s="7">
         <v>37681</v>
       </c>
-      <c r="B101" s="6">
+      <c r="B101" s="8">
         <v>0.17960657789052537</v>
       </c>
       <c r="CG101" s="1"/>
@@ -4982,10 +4997,10 @@
       <c r="QQ101" s="1"/>
     </row>
     <row r="102" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A102" s="5">
+      <c r="A102" s="7">
         <v>37712</v>
       </c>
-      <c r="B102" s="6">
+      <c r="B102" s="8">
         <v>0.17370103158576525</v>
       </c>
       <c r="CG102" s="1"/>
@@ -5033,10 +5048,10 @@
       <c r="QQ102" s="1"/>
     </row>
     <row r="103" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A103" s="5">
+      <c r="A103" s="7">
         <v>37742</v>
       </c>
-      <c r="B103" s="6">
+      <c r="B103" s="8">
         <v>0.17745962817797939</v>
       </c>
       <c r="CG103" s="1"/>
@@ -5085,10 +5100,10 @@
       <c r="QQ103" s="1"/>
     </row>
     <row r="104" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A104" s="5">
+      <c r="A104" s="7">
         <v>37773</v>
       </c>
-      <c r="B104" s="6">
+      <c r="B104" s="8">
         <v>0.17353423821042152</v>
       </c>
       <c r="CG104" s="1"/>
@@ -5138,10 +5153,10 @@
       <c r="QQ104" s="1"/>
     </row>
     <row r="105" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A105" s="5">
+      <c r="A105" s="7">
         <v>37803</v>
       </c>
-      <c r="B105" s="6">
+      <c r="B105" s="8">
         <v>0.16443232371464103</v>
       </c>
       <c r="CG105" s="1"/>
@@ -5191,10 +5206,10 @@
       <c r="QQ105" s="1"/>
     </row>
     <row r="106" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A106" s="5">
+      <c r="A106" s="7">
         <v>37834</v>
       </c>
-      <c r="B106" s="6">
+      <c r="B106" s="8">
         <v>0.16083606998584948</v>
       </c>
       <c r="CG106" s="1"/>
@@ -5245,10 +5260,10 @@
       <c r="QQ106" s="1"/>
     </row>
     <row r="107" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A107" s="5">
+      <c r="A107" s="7">
         <v>37865</v>
       </c>
-      <c r="B107" s="6">
+      <c r="B107" s="8">
         <v>0.19762447566023092</v>
       </c>
       <c r="CG107" s="1"/>
@@ -5303,10 +5318,10 @@
       <c r="RX107" s="1"/>
     </row>
     <row r="108" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A108" s="5">
+      <c r="A108" s="7">
         <v>37895</v>
       </c>
-      <c r="B108" s="6">
+      <c r="B108" s="8">
         <v>0.18706253495325156</v>
       </c>
       <c r="CG108" s="1"/>
@@ -5361,10 +5376,10 @@
       <c r="RX108" s="1"/>
     </row>
     <row r="109" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A109" s="5">
+      <c r="A109" s="7">
         <v>37926</v>
       </c>
-      <c r="B109" s="6">
+      <c r="B109" s="8">
         <v>0.18579912866791054</v>
       </c>
       <c r="CG109" s="1"/>
@@ -5421,10 +5436,10 @@
       <c r="RX109" s="1"/>
     </row>
     <row r="110" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A110" s="5">
+      <c r="A110" s="7">
         <v>37956</v>
       </c>
-      <c r="B110" s="6">
+      <c r="B110" s="8">
         <v>0.15228963728645464</v>
       </c>
       <c r="CG110" s="1"/>
@@ -5483,10 +5498,10 @@
       <c r="RX110" s="1"/>
     </row>
     <row r="111" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A111" s="5">
+      <c r="A111" s="7">
         <v>37987</v>
       </c>
-      <c r="B111" s="6">
+      <c r="B111" s="8">
         <v>0.14979423018271038</v>
       </c>
       <c r="CG111" s="1"/>
@@ -5545,10 +5560,10 @@
       <c r="RX111" s="1"/>
     </row>
     <row r="112" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A112" s="5">
+      <c r="A112" s="7">
         <v>38018</v>
       </c>
-      <c r="B112" s="6">
+      <c r="B112" s="8">
         <v>0.15531103806729979</v>
       </c>
       <c r="CG112" s="1"/>
@@ -5607,10 +5622,10 @@
       <c r="RX112" s="1"/>
     </row>
     <row r="113" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A113" s="5">
+      <c r="A113" s="7">
         <v>38047</v>
       </c>
-      <c r="B113" s="6">
+      <c r="B113" s="8">
         <v>0.15189953279944524</v>
       </c>
       <c r="CG113" s="1"/>
@@ -5671,10 +5686,10 @@
       <c r="RX113" s="1"/>
     </row>
     <row r="114" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A114" s="5">
+      <c r="A114" s="7">
         <v>38078</v>
       </c>
-      <c r="B114" s="6">
+      <c r="B114" s="8">
         <v>0.14238155308795486</v>
       </c>
       <c r="CG114" s="1"/>
@@ -5736,10 +5751,10 @@
       <c r="RX114" s="1"/>
     </row>
     <row r="115" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A115" s="5">
+      <c r="A115" s="7">
         <v>38108</v>
       </c>
-      <c r="B115" s="6">
+      <c r="B115" s="8">
         <v>0.13993688563245948</v>
       </c>
       <c r="CG115" s="1"/>
@@ -5812,10 +5827,10 @@
       <c r="RX115" s="1"/>
     </row>
     <row r="116" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A116" s="5">
+      <c r="A116" s="7">
         <v>38139</v>
       </c>
-      <c r="B116" s="6">
+      <c r="B116" s="8">
         <v>0.13205156859518685</v>
       </c>
       <c r="CG116" s="1"/>
@@ -5899,10 +5914,10 @@
       <c r="RX116" s="1"/>
     </row>
     <row r="117" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A117" s="5">
+      <c r="A117" s="7">
         <v>38169</v>
       </c>
-      <c r="B117" s="6">
+      <c r="B117" s="8">
         <v>0.1321356483644931</v>
       </c>
       <c r="CG117" s="1"/>
@@ -5988,10 +6003,10 @@
       <c r="RX117" s="1"/>
     </row>
     <row r="118" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A118" s="5">
+      <c r="A118" s="7">
         <v>38200</v>
       </c>
-      <c r="B118" s="6">
+      <c r="B118" s="8">
         <v>0.13235416398227642</v>
       </c>
       <c r="CG118" s="1"/>
@@ -6077,10 +6092,10 @@
       <c r="RX118" s="1"/>
     </row>
     <row r="119" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A119" s="5">
+      <c r="A119" s="7">
         <v>38231</v>
       </c>
-      <c r="B119" s="6">
+      <c r="B119" s="8">
         <v>0.14198841003714582</v>
       </c>
       <c r="CG119" s="1"/>
@@ -6166,10 +6181,10 @@
       <c r="RX119" s="1"/>
     </row>
     <row r="120" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A120" s="5">
+      <c r="A120" s="7">
         <v>38261</v>
       </c>
-      <c r="B120" s="6">
+      <c r="B120" s="8">
         <v>0.14054340020098038</v>
       </c>
       <c r="CG120" s="1"/>
@@ -6255,10 +6270,10 @@
       <c r="RX120" s="1"/>
     </row>
     <row r="121" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A121" s="5">
+      <c r="A121" s="7">
         <v>38292</v>
       </c>
-      <c r="B121" s="6">
+      <c r="B121" s="8">
         <v>0.13208337856049901</v>
       </c>
       <c r="CG121" s="1"/>
@@ -6345,10 +6360,10 @@
       <c r="RX121" s="1"/>
     </row>
     <row r="122" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A122" s="5">
+      <c r="A122" s="7">
         <v>38322</v>
       </c>
-      <c r="B122" s="6">
+      <c r="B122" s="8">
         <v>0.13722393226951568</v>
       </c>
       <c r="CG122" s="1"/>
@@ -6435,10 +6450,10 @@
       <c r="RX122" s="1"/>
     </row>
     <row r="123" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A123" s="5">
+      <c r="A123" s="7">
         <v>38353</v>
       </c>
-      <c r="B123" s="6">
+      <c r="B123" s="8">
         <v>0.13998031470880479</v>
       </c>
       <c r="CG123" s="1"/>
@@ -6525,10 +6540,10 @@
       <c r="RX123" s="1"/>
     </row>
     <row r="124" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A124" s="5">
+      <c r="A124" s="7">
         <v>38384</v>
       </c>
-      <c r="B124" s="6">
+      <c r="B124" s="8">
         <v>0.14381330437458539</v>
       </c>
       <c r="CG124" s="1"/>
@@ -6617,10 +6632,10 @@
       <c r="RX124" s="1"/>
     </row>
     <row r="125" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A125" s="5">
+      <c r="A125" s="7">
         <v>38412</v>
       </c>
-      <c r="B125" s="6">
+      <c r="B125" s="8">
         <v>0.13883886128708484</v>
       </c>
       <c r="CG125" s="1"/>
@@ -6709,10 +6724,10 @@
       <c r="RX125" s="1"/>
     </row>
     <row r="126" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A126" s="5">
+      <c r="A126" s="7">
         <v>38443</v>
       </c>
-      <c r="B126" s="6">
+      <c r="B126" s="8">
         <v>0.14223096597630486</v>
       </c>
       <c r="CG126" s="1"/>
@@ -6801,10 +6816,10 @@
       <c r="RX126" s="1"/>
     </row>
     <row r="127" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A127" s="5">
+      <c r="A127" s="7">
         <v>38473</v>
       </c>
-      <c r="B127" s="6">
+      <c r="B127" s="8">
         <v>0.15130856651883109</v>
       </c>
       <c r="CG127" s="1"/>
@@ -6894,10 +6909,10 @@
       <c r="RX127" s="1"/>
     </row>
     <row r="128" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A128" s="5">
+      <c r="A128" s="7">
         <v>38504</v>
       </c>
-      <c r="B128" s="6">
+      <c r="B128" s="8">
         <v>0.17613645867084826</v>
       </c>
       <c r="CG128" s="1"/>
@@ -6988,10 +7003,10 @@
       <c r="RX128" s="1"/>
     </row>
     <row r="129" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A129" s="5">
+      <c r="A129" s="7">
         <v>38534</v>
       </c>
-      <c r="B129" s="6">
+      <c r="B129" s="8">
         <v>0.17526795031368764</v>
       </c>
       <c r="CG129" s="1"/>
@@ -7082,10 +7097,10 @@
       <c r="RX129" s="1"/>
     </row>
     <row r="130" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A130" s="5">
+      <c r="A130" s="7">
         <v>38565</v>
       </c>
-      <c r="B130" s="6">
+      <c r="B130" s="8">
         <v>0.17356897074457586</v>
       </c>
       <c r="CG130" s="1"/>
@@ -7176,10 +7191,10 @@
       <c r="RX130" s="1"/>
     </row>
     <row r="131" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A131" s="5">
+      <c r="A131" s="7">
         <v>38596</v>
       </c>
-      <c r="B131" s="6">
+      <c r="B131" s="8">
         <v>0.13496571144618535</v>
       </c>
       <c r="CG131" s="1"/>
@@ -7270,10 +7285,10 @@
       <c r="RX131" s="1"/>
     </row>
     <row r="132" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A132" s="5">
+      <c r="A132" s="7">
         <v>38626</v>
       </c>
-      <c r="B132" s="6">
+      <c r="B132" s="8">
         <v>0.13393339678506488</v>
       </c>
       <c r="CG132" s="1"/>
@@ -7364,10 +7379,10 @@
       <c r="RX132" s="1"/>
     </row>
     <row r="133" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A133" s="5">
+      <c r="A133" s="7">
         <v>38657</v>
       </c>
-      <c r="B133" s="6">
+      <c r="B133" s="8">
         <v>0.13831045015123039</v>
       </c>
       <c r="CG133" s="1"/>
@@ -7458,10 +7473,10 @@
       <c r="RX133" s="1"/>
     </row>
     <row r="134" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A134" s="5">
+      <c r="A134" s="7">
         <v>38687</v>
       </c>
-      <c r="B134" s="6">
+      <c r="B134" s="8">
         <v>0.12603299570326587</v>
       </c>
       <c r="CG134" s="1"/>
@@ -7552,10 +7567,10 @@
       <c r="RX134" s="1"/>
     </row>
     <row r="135" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A135" s="5">
+      <c r="A135" s="7">
         <v>38718</v>
       </c>
-      <c r="B135" s="6">
+      <c r="B135" s="8">
         <v>0.12251013261185581</v>
       </c>
       <c r="CG135" s="1"/>
@@ -7646,10 +7661,10 @@
       <c r="RX135" s="1"/>
     </row>
     <row r="136" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A136" s="5">
+      <c r="A136" s="7">
         <v>38749</v>
       </c>
-      <c r="B136" s="6">
+      <c r="B136" s="8">
         <v>0.11689155988668461</v>
       </c>
       <c r="CG136" s="1"/>
@@ -7740,10 +7755,10 @@
       <c r="RX136" s="1"/>
     </row>
     <row r="137" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A137" s="5">
+      <c r="A137" s="7">
         <v>38777</v>
       </c>
-      <c r="B137" s="6">
+      <c r="B137" s="8">
         <v>0.11182793411322625</v>
       </c>
       <c r="CG137" s="1"/>
@@ -7834,10 +7849,10 @@
       <c r="RX137" s="1"/>
     </row>
     <row r="138" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A138" s="5">
+      <c r="A138" s="7">
         <v>38808</v>
       </c>
-      <c r="B138" s="6">
+      <c r="B138" s="8">
         <v>0.1062966817216436</v>
       </c>
       <c r="CG138" s="1"/>
@@ -7928,10 +7943,10 @@
       <c r="RX138" s="1"/>
     </row>
     <row r="139" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A139" s="5">
+      <c r="A139" s="7">
         <v>38838</v>
       </c>
-      <c r="B139" s="6">
+      <c r="B139" s="8">
         <v>0.10685897585166657</v>
       </c>
       <c r="CG139" s="1"/>
@@ -8022,10 +8037,10 @@
       <c r="RX139" s="1"/>
     </row>
     <row r="140" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A140" s="5">
+      <c r="A140" s="7">
         <v>38869</v>
       </c>
-      <c r="B140" s="6">
+      <c r="B140" s="8">
         <v>0.10321059015113987</v>
       </c>
       <c r="CG140" s="1"/>
@@ -8116,10 +8131,10 @@
       <c r="RX140" s="1"/>
     </row>
     <row r="141" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A141" s="5">
+      <c r="A141" s="7">
         <v>38899</v>
       </c>
-      <c r="B141" s="6">
+      <c r="B141" s="8">
         <v>0.1042737605249823</v>
       </c>
       <c r="CG141" s="1"/>
@@ -8210,10 +8225,10 @@
       <c r="RX141" s="1"/>
     </row>
     <row r="142" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A142" s="5">
+      <c r="A142" s="7">
         <v>38930</v>
       </c>
-      <c r="B142" s="6">
+      <c r="B142" s="8">
         <v>9.9191823334113305E-2</v>
       </c>
       <c r="CG142" s="1"/>
@@ -8304,10 +8319,10 @@
       <c r="RX142" s="1"/>
     </row>
     <row r="143" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A143" s="5">
+      <c r="A143" s="7">
         <v>38961</v>
       </c>
-      <c r="B143" s="6">
+      <c r="B143" s="8">
         <v>9.7977952179741312E-2</v>
       </c>
       <c r="CG143" s="1"/>
@@ -8398,10 +8413,10 @@
       <c r="RX143" s="1"/>
     </row>
     <row r="144" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A144" s="5">
+      <c r="A144" s="7">
         <v>38991</v>
       </c>
-      <c r="B144" s="6">
+      <c r="B144" s="8">
         <v>9.5864636506678785E-2</v>
       </c>
       <c r="CG144" s="1"/>
@@ -8492,10 +8507,10 @@
       <c r="RX144" s="1"/>
     </row>
     <row r="145" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A145" s="5">
+      <c r="A145" s="7">
         <v>39022</v>
       </c>
-      <c r="B145" s="6">
+      <c r="B145" s="8">
         <v>8.8506947539146508E-2</v>
       </c>
       <c r="CG145" s="1"/>
@@ -8586,10 +8601,10 @@
       <c r="RX145" s="1"/>
     </row>
     <row r="146" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A146" s="5">
+      <c r="A146" s="7">
         <v>39052</v>
       </c>
-      <c r="B146" s="6">
+      <c r="B146" s="8">
         <v>8.2991557693164242E-2</v>
       </c>
       <c r="CG146" s="1"/>
@@ -8680,10 +8695,10 @@
       <c r="RX146" s="1"/>
     </row>
     <row r="147" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A147" s="5">
+      <c r="A147" s="7">
         <v>39083</v>
       </c>
-      <c r="B147" s="6">
+      <c r="B147" s="8">
         <v>7.7215118349207135E-2</v>
       </c>
       <c r="CG147" s="1"/>
@@ -8774,10 +8789,10 @@
       <c r="RX147" s="1"/>
     </row>
     <row r="148" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A148" s="5">
+      <c r="A148" s="7">
         <v>39114</v>
       </c>
-      <c r="B148" s="6">
+      <c r="B148" s="8">
         <v>7.9397037241236174E-2</v>
       </c>
       <c r="CG148" s="1"/>
@@ -8868,10 +8883,10 @@
       <c r="RX148" s="1"/>
     </row>
     <row r="149" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A149" s="5">
+      <c r="A149" s="7">
         <v>39142</v>
       </c>
-      <c r="B149" s="6">
+      <c r="B149" s="8">
         <v>9.5585255682960557E-2</v>
       </c>
       <c r="CG149" s="1"/>
@@ -8962,10 +8977,10 @@
       <c r="RX149" s="1"/>
     </row>
     <row r="150" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A150" s="5">
+      <c r="A150" s="7">
         <v>39173</v>
       </c>
-      <c r="B150" s="6">
+      <c r="B150" s="8">
         <v>8.580606474485139E-2</v>
       </c>
       <c r="CG150" s="1"/>
@@ -9056,10 +9071,10 @@
       <c r="RX150" s="1"/>
     </row>
     <row r="151" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A151" s="5">
+      <c r="A151" s="7">
         <v>39203</v>
       </c>
-      <c r="B151" s="6">
+      <c r="B151" s="8">
         <v>8.1207326443699546E-2</v>
       </c>
       <c r="CG151" s="1"/>
@@ -9150,10 +9165,10 @@
       <c r="RX151" s="1"/>
     </row>
     <row r="152" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A152" s="5">
+      <c r="A152" s="7">
         <v>39234</v>
       </c>
-      <c r="B152" s="6">
+      <c r="B152" s="8">
         <v>8.2961482672590375E-2</v>
       </c>
       <c r="CG152" s="1"/>
@@ -9244,10 +9259,10 @@
       <c r="RX152" s="1"/>
     </row>
     <row r="153" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A153" s="5">
+      <c r="A153" s="7">
         <v>39264</v>
       </c>
-      <c r="B153" s="6">
+      <c r="B153" s="8">
         <v>8.5322650599013228E-2</v>
       </c>
       <c r="CG153" s="1"/>
@@ -9338,10 +9353,10 @@
       <c r="RX153" s="1"/>
     </row>
     <row r="154" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A154" s="5">
+      <c r="A154" s="7">
         <v>39295</v>
       </c>
-      <c r="B154" s="6">
+      <c r="B154" s="8">
         <v>8.5340133244383914E-2</v>
       </c>
       <c r="CG154" s="1"/>
@@ -9432,10 +9447,10 @@
       <c r="RX154" s="1"/>
     </row>
     <row r="155" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A155" s="5">
+      <c r="A155" s="7">
         <v>39326</v>
       </c>
-      <c r="B155" s="6">
+      <c r="B155" s="8">
         <v>8.8928884093107091E-2</v>
       </c>
       <c r="CG155" s="1"/>
@@ -9526,10 +9541,10 @@
       <c r="RX155" s="1"/>
     </row>
     <row r="156" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A156" s="5">
+      <c r="A156" s="7">
         <v>39356</v>
       </c>
-      <c r="B156" s="6">
+      <c r="B156" s="8">
         <v>8.7744511396229033E-2</v>
       </c>
       <c r="CG156" s="1"/>
@@ -9620,10 +9635,10 @@
       <c r="RX156" s="1"/>
     </row>
     <row r="157" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A157" s="5">
+      <c r="A157" s="7">
         <v>39387</v>
       </c>
-      <c r="B157" s="6">
+      <c r="B157" s="8">
         <v>9.3737830955098772E-2</v>
       </c>
       <c r="CG157" s="1"/>
@@ -9714,10 +9729,10 @@
       <c r="RX157" s="1"/>
     </row>
     <row r="158" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A158" s="5">
+      <c r="A158" s="7">
         <v>39417</v>
       </c>
-      <c r="B158" s="6">
+      <c r="B158" s="8">
         <v>8.671239907127623E-2</v>
       </c>
       <c r="CG158" s="1"/>
@@ -9808,10 +9823,10 @@
       <c r="RX158" s="1"/>
     </row>
     <row r="159" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A159" s="5">
+      <c r="A159" s="7">
         <v>39448</v>
       </c>
-      <c r="B159" s="6">
+      <c r="B159" s="8">
         <v>9.417152259727482E-2</v>
       </c>
       <c r="CG159" s="1"/>
@@ -9902,10 +9917,10 @@
       <c r="RX159" s="1"/>
     </row>
     <row r="160" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A160" s="5">
+      <c r="A160" s="7">
         <v>39479</v>
       </c>
-      <c r="B160" s="6">
+      <c r="B160" s="8">
         <v>9.3871674916660583E-2</v>
       </c>
       <c r="CG160" s="1"/>
@@ -9996,10 +10011,10 @@
       <c r="RX160" s="1"/>
     </row>
     <row r="161" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A161" s="5">
+      <c r="A161" s="7">
         <v>39508</v>
       </c>
-      <c r="B161" s="6">
+      <c r="B161" s="8">
         <v>9.5682797110982654E-2</v>
       </c>
       <c r="CG161" s="1"/>
@@ -10090,10 +10105,10 @@
       <c r="RX161" s="1"/>
     </row>
     <row r="162" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A162" s="5">
+      <c r="A162" s="7">
         <v>39539</v>
       </c>
-      <c r="B162" s="6">
+      <c r="B162" s="8">
         <v>8.9221726200208809E-2</v>
       </c>
       <c r="CG162" s="1"/>
@@ -10184,10 +10199,10 @@
       <c r="RX162" s="1"/>
     </row>
     <row r="163" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A163" s="5">
+      <c r="A163" s="7">
         <v>39569</v>
       </c>
-      <c r="B163" s="6">
+      <c r="B163" s="8">
         <v>8.5276870884392231E-2</v>
       </c>
       <c r="CG163" s="1"/>
@@ -10278,10 +10293,10 @@
       <c r="RX163" s="1"/>
     </row>
     <row r="164" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A164" s="5">
+      <c r="A164" s="7">
         <v>39600</v>
       </c>
-      <c r="B164" s="6">
+      <c r="B164" s="8">
         <v>9.0760799631218497E-2</v>
       </c>
       <c r="CG164" s="1"/>
@@ -10372,10 +10387,10 @@
       <c r="RX164" s="1"/>
     </row>
     <row r="165" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A165" s="5">
+      <c r="A165" s="7">
         <v>39630</v>
       </c>
-      <c r="B165" s="6">
+      <c r="B165" s="8">
         <v>9.0094041432956906E-2</v>
       </c>
       <c r="CG165" s="1"/>
@@ -10466,10 +10481,10 @@
       <c r="RX165" s="1"/>
     </row>
     <row r="166" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A166" s="5">
+      <c r="A166" s="7">
         <v>39661</v>
       </c>
-      <c r="B166" s="6">
+      <c r="B166" s="8">
         <v>9.2978334258690121E-2</v>
       </c>
       <c r="CG166" s="1"/>
@@ -10560,10 +10575,10 @@
       <c r="RX166" s="1"/>
     </row>
     <row r="167" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A167" s="5">
+      <c r="A167" s="7">
         <v>39692</v>
       </c>
-      <c r="B167" s="6">
+      <c r="B167" s="8">
         <v>0.1049190744132513</v>
       </c>
       <c r="CG167" s="1"/>
@@ -10654,10 +10669,10 @@
       <c r="RX167" s="1"/>
     </row>
     <row r="168" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A168" s="5">
+      <c r="A168" s="7">
         <v>39722</v>
       </c>
-      <c r="B168" s="6">
+      <c r="B168" s="8">
         <v>0.1150227873640902</v>
       </c>
       <c r="CG168" s="1"/>
@@ -10748,10 +10763,10 @@
       <c r="RX168" s="1"/>
     </row>
     <row r="169" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A169" s="5">
+      <c r="A169" s="7">
         <v>39753</v>
       </c>
-      <c r="B169" s="6">
+      <c r="B169" s="8">
         <v>0.12713618920136005</v>
       </c>
       <c r="CG169" s="1"/>
@@ -10842,10 +10857,10 @@
       <c r="RX169" s="1"/>
     </row>
     <row r="170" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A170" s="5">
+      <c r="A170" s="7">
         <v>39783</v>
       </c>
-      <c r="B170" s="6">
+      <c r="B170" s="8">
         <v>0.14219604354597082</v>
       </c>
       <c r="CG170" s="1"/>
@@ -10936,10 +10951,10 @@
       <c r="RX170" s="1"/>
     </row>
     <row r="171" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A171" s="5">
+      <c r="A171" s="7">
         <v>39814</v>
       </c>
-      <c r="B171" s="6">
+      <c r="B171" s="8">
         <v>0.13409152093551951</v>
       </c>
       <c r="CG171" s="1"/>
@@ -11030,10 +11045,10 @@
       <c r="RX171" s="1"/>
     </row>
     <row r="172" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A172" s="5">
+      <c r="A172" s="7">
         <v>39845</v>
       </c>
-      <c r="B172" s="6">
+      <c r="B172" s="8">
         <v>0.1323173344014103</v>
       </c>
       <c r="CG172" s="1"/>
@@ -11124,10 +11139,10 @@
       <c r="RX172" s="1"/>
     </row>
     <row r="173" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A173" s="5">
+      <c r="A173" s="7">
         <v>39873</v>
       </c>
-      <c r="B173" s="6">
+      <c r="B173" s="8">
         <v>0.12184780792693525</v>
       </c>
       <c r="CG173" s="1"/>
@@ -11218,10 +11233,10 @@
       <c r="RX173" s="1"/>
     </row>
     <row r="174" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A174" s="5">
+      <c r="A174" s="7">
         <v>39904</v>
       </c>
-      <c r="B174" s="6">
+      <c r="B174" s="8">
         <v>0.1088401890456267</v>
       </c>
       <c r="CG174" s="1"/>
@@ -11312,10 +11327,10 @@
       <c r="RX174" s="1"/>
     </row>
     <row r="175" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A175" s="5">
+      <c r="A175" s="7">
         <v>39934</v>
       </c>
-      <c r="B175" s="6">
+      <c r="B175" s="8">
         <v>0.10207538732969924</v>
       </c>
       <c r="CG175" s="1"/>
@@ -11406,10 +11421,10 @@
       <c r="RX175" s="1"/>
     </row>
     <row r="176" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A176" s="5">
+      <c r="A176" s="7">
         <v>39965</v>
       </c>
-      <c r="B176" s="6">
+      <c r="B176" s="8">
         <v>9.0431157247827659E-2</v>
       </c>
       <c r="CG176" s="1"/>
@@ -11500,10 +11515,10 @@
       <c r="RX176" s="1"/>
     </row>
     <row r="177" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A177" s="5">
+      <c r="A177" s="7">
         <v>39995</v>
       </c>
-      <c r="B177" s="6">
+      <c r="B177" s="8">
         <v>8.8254360455356951E-2</v>
       </c>
       <c r="CG177" s="1"/>
@@ -11594,10 +11609,10 @@
       <c r="RX177" s="1"/>
     </row>
     <row r="178" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A178" s="5">
+      <c r="A178" s="7">
         <v>40026</v>
       </c>
-      <c r="B178" s="6">
+      <c r="B178" s="8">
         <v>8.5062467132288211E-2</v>
       </c>
       <c r="CG178" s="1"/>
@@ -11688,10 +11703,10 @@
       <c r="RX178" s="1"/>
     </row>
     <row r="179" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A179" s="5">
+      <c r="A179" s="7">
         <v>40057</v>
       </c>
-      <c r="B179" s="6">
+      <c r="B179" s="8">
         <v>8.194495980792163E-2</v>
       </c>
       <c r="CG179" s="1"/>
@@ -11782,10 +11797,10 @@
       <c r="RX179" s="1"/>
     </row>
     <row r="180" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A180" s="5">
+      <c r="A180" s="7">
         <v>40087</v>
       </c>
-      <c r="B180" s="6">
+      <c r="B180" s="8">
         <v>8.3103148537463978E-2</v>
       </c>
       <c r="CG180" s="1"/>
@@ -11876,10 +11891,10 @@
       <c r="RX180" s="1"/>
     </row>
     <row r="181" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A181" s="5">
+      <c r="A181" s="7">
         <v>40118</v>
       </c>
-      <c r="B181" s="6">
+      <c r="B181" s="8">
         <v>8.4939307901060079E-2</v>
       </c>
       <c r="CG181" s="1"/>
@@ -11970,10 +11985,10 @@
       <c r="RX181" s="1"/>
     </row>
     <row r="182" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A182" s="5">
+      <c r="A182" s="7">
         <v>40148</v>
       </c>
-      <c r="B182" s="6">
+      <c r="B182" s="8">
         <v>9.1998835222545483E-2</v>
       </c>
       <c r="CG182" s="1"/>
@@ -12064,10 +12079,10 @@
       <c r="RX182" s="1"/>
     </row>
     <row r="183" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A183" s="5">
+      <c r="A183" s="7">
         <v>40179</v>
       </c>
-      <c r="B183" s="6">
+      <c r="B183" s="8">
         <v>9.4406445060834981E-2</v>
       </c>
       <c r="CG183" s="1"/>
@@ -12158,10 +12173,10 @@
       <c r="RX183" s="1"/>
     </row>
     <row r="184" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A184" s="5">
+      <c r="A184" s="7">
         <v>40210</v>
       </c>
-      <c r="B184" s="6">
+      <c r="B184" s="8">
         <v>9.677333010017547E-2</v>
       </c>
       <c r="CG184" s="1"/>
@@ -12252,10 +12267,10 @@
       <c r="RX184" s="1"/>
     </row>
     <row r="185" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A185" s="5">
+      <c r="A185" s="7">
         <v>40238</v>
       </c>
-      <c r="B185" s="6">
+      <c r="B185" s="8">
         <v>0.10525014956324957</v>
       </c>
       <c r="CG185" s="1"/>
@@ -12346,10 +12361,10 @@
       <c r="RX185" s="1"/>
     </row>
     <row r="186" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A186" s="5">
+      <c r="A186" s="7">
         <v>40269</v>
       </c>
-      <c r="B186" s="6">
+      <c r="B186" s="8">
         <v>0.10079451028425426</v>
       </c>
       <c r="CG186" s="1"/>
@@ -12440,10 +12455,10 @@
       <c r="RX186" s="1"/>
     </row>
     <row r="187" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A187" s="5">
+      <c r="A187" s="7">
         <v>40299</v>
       </c>
-      <c r="B187" s="6">
+      <c r="B187" s="8">
         <v>9.7475443102761017E-2</v>
       </c>
       <c r="CG187" s="1"/>
@@ -12534,10 +12549,10 @@
       <c r="RX187" s="1"/>
     </row>
     <row r="188" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A188" s="5">
+      <c r="A188" s="7">
         <v>40330</v>
       </c>
-      <c r="B188" s="6">
+      <c r="B188" s="8">
         <v>0.10575656830811714</v>
       </c>
       <c r="CG188" s="1"/>
@@ -12628,10 +12643,10 @@
       <c r="RX188" s="1"/>
     </row>
     <row r="189" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A189" s="5">
+      <c r="A189" s="7">
         <v>40360</v>
       </c>
-      <c r="B189" s="6">
+      <c r="B189" s="8">
         <v>0.10532947410949854</v>
       </c>
       <c r="CG189" s="1"/>
@@ -12722,10 +12737,10 @@
       <c r="RX189" s="1"/>
     </row>
     <row r="190" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A190" s="5">
+      <c r="A190" s="7">
         <v>40391</v>
       </c>
-      <c r="B190" s="6">
+      <c r="B190" s="8">
         <v>0.10550581781341299</v>
       </c>
       <c r="CG190" s="1"/>
@@ -12816,10 +12831,10 @@
       <c r="RX190" s="1"/>
     </row>
     <row r="191" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A191" s="5">
+      <c r="A191" s="7">
         <v>40422</v>
       </c>
-      <c r="B191" s="6">
+      <c r="B191" s="8">
         <v>0.10964076002117032</v>
       </c>
       <c r="CG191" s="1"/>
@@ -12910,10 +12925,10 @@
       <c r="RX191" s="1"/>
     </row>
     <row r="192" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A192" s="5">
+      <c r="A192" s="7">
         <v>40452</v>
       </c>
-      <c r="B192" s="6">
+      <c r="B192" s="8">
         <v>0.10513412866678648</v>
       </c>
       <c r="CG192" s="1"/>
@@ -13004,10 +13019,10 @@
       <c r="RX192" s="1"/>
     </row>
     <row r="193" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A193" s="5">
+      <c r="A193" s="7">
         <v>40483</v>
       </c>
-      <c r="B193" s="6">
+      <c r="B193" s="8">
         <v>0.10473580686784892</v>
       </c>
       <c r="CG193" s="1"/>
@@ -13098,10 +13113,10 @@
       <c r="RX193" s="1"/>
     </row>
     <row r="194" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A194" s="5">
+      <c r="A194" s="7">
         <v>40513</v>
       </c>
-      <c r="B194" s="6">
+      <c r="B194" s="8">
         <v>9.4346589276028653E-2</v>
       </c>
       <c r="CG194" s="1"/>
@@ -13192,10 +13207,10 @@
       <c r="RX194" s="1"/>
     </row>
     <row r="195" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A195" s="5">
+      <c r="A195" s="7">
         <v>40544</v>
       </c>
-      <c r="B195" s="6">
+      <c r="B195" s="8">
         <v>9.5407238018712093E-2</v>
       </c>
       <c r="CG195" s="1"/>
@@ -13286,10 +13301,10 @@
       <c r="RX195" s="1"/>
     </row>
     <row r="196" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A196" s="5">
+      <c r="A196" s="7">
         <v>40575</v>
       </c>
-      <c r="B196" s="6">
+      <c r="B196" s="8">
         <v>9.3390806727688513E-2</v>
       </c>
       <c r="CG196" s="1"/>
@@ -13380,10 +13395,10 @@
       <c r="RX196" s="1"/>
     </row>
     <row r="197" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A197" s="5">
+      <c r="A197" s="7">
         <v>40603</v>
       </c>
-      <c r="B197" s="6">
+      <c r="B197" s="8">
         <v>9.3441141720405185E-2</v>
       </c>
       <c r="CG197" s="1"/>
@@ -13474,10 +13489,10 @@
       <c r="RX197" s="1"/>
     </row>
     <row r="198" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A198" s="5">
+      <c r="A198" s="7">
         <v>40634</v>
       </c>
-      <c r="B198" s="6">
+      <c r="B198" s="8">
         <v>9.3643791643206381E-2</v>
       </c>
       <c r="CG198" s="1"/>
@@ -13568,10 +13583,10 @@
       <c r="RX198" s="1"/>
     </row>
     <row r="199" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A199" s="5">
+      <c r="A199" s="7">
         <v>40664</v>
       </c>
-      <c r="B199" s="6">
+      <c r="B199" s="8">
         <v>0.10032836280974664</v>
       </c>
       <c r="CG199" s="1"/>
@@ -13662,10 +13677,10 @@
       <c r="RX199" s="1"/>
     </row>
     <row r="200" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A200" s="5">
+      <c r="A200" s="7">
         <v>40695</v>
       </c>
-      <c r="B200" s="6">
+      <c r="B200" s="8">
         <v>9.9388836279557288E-2</v>
       </c>
       <c r="CG200" s="1"/>
@@ -13756,10 +13771,10 @@
       <c r="RX200" s="1"/>
     </row>
     <row r="201" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A201" s="5">
+      <c r="A201" s="7">
         <v>40725</v>
       </c>
-      <c r="B201" s="6">
+      <c r="B201" s="8">
         <v>0.10538607103302287</v>
       </c>
       <c r="CG201" s="1"/>
@@ -13850,10 +13865,10 @@
       <c r="RX201" s="1"/>
     </row>
     <row r="202" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A202" s="5">
+      <c r="A202" s="7">
         <v>40756</v>
       </c>
-      <c r="B202" s="6">
+      <c r="B202" s="8">
         <v>0.11212100068797148</v>
       </c>
       <c r="CG202" s="1"/>
@@ -13944,10 +13959,10 @@
       <c r="RX202" s="1"/>
     </row>
     <row r="203" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A203" s="5">
+      <c r="A203" s="7">
         <v>40787</v>
       </c>
-      <c r="B203" s="6">
+      <c r="B203" s="8">
         <v>0.110785960833959</v>
       </c>
       <c r="CG203" s="1"/>
@@ -14038,10 +14053,10 @@
       <c r="RX203" s="1"/>
     </row>
     <row r="204" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A204" s="5">
+      <c r="A204" s="7">
         <v>40817</v>
       </c>
-      <c r="B204" s="6">
+      <c r="B204" s="8">
         <v>0.10360612595722082</v>
       </c>
       <c r="CG204" s="1"/>
@@ -14132,10 +14147,10 @@
       <c r="RX204" s="1"/>
     </row>
     <row r="205" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A205" s="5">
+      <c r="A205" s="7">
         <v>40848</v>
       </c>
-      <c r="B205" s="6">
+      <c r="B205" s="8">
         <v>0.10488449858019411</v>
       </c>
       <c r="CG205" s="1"/>
@@ -14226,10 +14241,10 @@
       <c r="RX205" s="1"/>
     </row>
     <row r="206" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A206" s="5">
+      <c r="A206" s="7">
         <v>40878</v>
       </c>
-      <c r="B206" s="6">
+      <c r="B206" s="8">
         <v>0.10009455642023066</v>
       </c>
       <c r="CG206" s="1"/>
@@ -14283,7 +14298,7 @@
       <c r="JL206" s="1"/>
       <c r="JW206" s="1"/>
       <c r="KH206" s="1"/>
-      <c r="KJ206" s="3"/>
+      <c r="KJ206" s="5"/>
       <c r="KS206" s="1"/>
       <c r="LD206" s="1"/>
       <c r="LE206" s="1"/>
@@ -14321,10 +14336,10 @@
       <c r="RX206" s="1"/>
     </row>
     <row r="207" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A207" s="5">
+      <c r="A207" s="7">
         <v>40909</v>
       </c>
-      <c r="B207" s="6">
+      <c r="B207" s="8">
         <v>9.6997483527202721E-2</v>
       </c>
       <c r="CG207" s="1"/>
@@ -14391,7 +14406,7 @@
       <c r="LM207" s="1"/>
       <c r="LO207" s="1"/>
       <c r="LZ207" s="1"/>
-      <c r="MB207" s="3"/>
+      <c r="MB207" s="5"/>
       <c r="MK207" s="1"/>
       <c r="MV207" s="1"/>
       <c r="NG207" s="1"/>
@@ -14416,10 +14431,10 @@
       <c r="RX207" s="1"/>
     </row>
     <row r="208" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A208" s="5">
+      <c r="A208" s="7">
         <v>40940</v>
       </c>
-      <c r="B208" s="6">
+      <c r="B208" s="8">
         <v>9.0887604642450229E-2</v>
       </c>
       <c r="CG208" s="1"/>
@@ -14474,7 +14489,7 @@
       <c r="JW208" s="1"/>
       <c r="KH208" s="1"/>
       <c r="KS208" s="1"/>
-      <c r="KU208" s="3"/>
+      <c r="KU208" s="5"/>
       <c r="LD208" s="1"/>
       <c r="LE208" s="1"/>
       <c r="LF208" s="1"/>
@@ -14488,13 +14503,13 @@
       <c r="LO208" s="1"/>
       <c r="LZ208" s="1"/>
       <c r="MK208" s="1"/>
-      <c r="MM208" s="3"/>
+      <c r="MM208" s="5"/>
       <c r="MV208" s="1"/>
-      <c r="MX208" s="3"/>
+      <c r="MX208" s="5"/>
       <c r="NG208" s="1"/>
       <c r="NR208" s="1"/>
       <c r="OC208" s="1"/>
-      <c r="OE208" s="3"/>
+      <c r="OE208" s="5"/>
       <c r="ON208" s="1"/>
       <c r="OY208" s="1"/>
       <c r="PJ208" s="1"/>
@@ -14514,10 +14529,10 @@
       <c r="RX208" s="1"/>
     </row>
     <row r="209" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A209" s="5">
+      <c r="A209" s="7">
         <v>40969</v>
       </c>
-      <c r="B209" s="6">
+      <c r="B209" s="8">
         <v>8.7800298912843522E-2</v>
       </c>
       <c r="CG209" s="1"/>
@@ -14574,7 +14589,7 @@
       <c r="KS209" s="1"/>
       <c r="LD209" s="1"/>
       <c r="LE209" s="1"/>
-      <c r="LF209" s="3"/>
+      <c r="LF209" s="5"/>
       <c r="LG209" s="1"/>
       <c r="LH209" s="1"/>
       <c r="LI209" s="1"/>
@@ -14592,7 +14607,7 @@
       <c r="ON209" s="1"/>
       <c r="OY209" s="1"/>
       <c r="PJ209" s="1"/>
-      <c r="PL209" s="3"/>
+      <c r="PL209" s="5"/>
       <c r="PU209" s="1"/>
       <c r="PV209" s="1"/>
       <c r="PW209" s="1"/>
@@ -14609,10 +14624,10 @@
       <c r="RX209" s="1"/>
     </row>
     <row r="210" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A210" s="5">
+      <c r="A210" s="7">
         <v>41000</v>
       </c>
-      <c r="B210" s="6">
+      <c r="B210" s="8">
         <v>9.5810214550751407E-2</v>
       </c>
       <c r="CG210" s="1"/>
@@ -14678,18 +14693,18 @@
       <c r="LL210" s="1"/>
       <c r="LM210" s="1"/>
       <c r="LO210" s="1"/>
-      <c r="LQ210" s="3"/>
+      <c r="LQ210" s="5"/>
       <c r="LZ210" s="1"/>
       <c r="MK210" s="1"/>
       <c r="MV210" s="1"/>
       <c r="NG210" s="1"/>
-      <c r="NI210" s="3"/>
+      <c r="NI210" s="5"/>
       <c r="NR210" s="1"/>
-      <c r="NT210" s="3"/>
+      <c r="NT210" s="5"/>
       <c r="OC210" s="1"/>
       <c r="ON210" s="1"/>
       <c r="OY210" s="1"/>
-      <c r="PA210" s="3"/>
+      <c r="PA210" s="5"/>
       <c r="PJ210" s="1"/>
       <c r="PU210" s="1"/>
       <c r="PV210" s="1"/>
@@ -14707,10 +14722,10 @@
       <c r="RX210" s="1"/>
     </row>
     <row r="211" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A211" s="5">
+      <c r="A211" s="7">
         <v>41030</v>
       </c>
-      <c r="B211" s="6">
+      <c r="B211" s="8">
         <v>0.10515093938008996</v>
       </c>
       <c r="CG211" s="1"/>
@@ -14801,10 +14816,10 @@
       <c r="RX211" s="1"/>
     </row>
     <row r="212" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A212" s="5">
+      <c r="A212" s="7">
         <v>41061</v>
       </c>
-      <c r="B212" s="6">
+      <c r="B212" s="8">
         <v>9.0817328850805651E-2</v>
       </c>
       <c r="CG212" s="1"/>
@@ -14877,7 +14892,7 @@
       <c r="NR212" s="1"/>
       <c r="OC212" s="1"/>
       <c r="ON212" s="1"/>
-      <c r="OP212" s="3"/>
+      <c r="OP212" s="5"/>
       <c r="OY212" s="1"/>
       <c r="PJ212" s="1"/>
       <c r="PU212" s="1"/>
@@ -14896,10 +14911,10 @@
       <c r="RX212" s="1"/>
     </row>
     <row r="213" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A213" s="5">
+      <c r="A213" s="7">
         <v>41091</v>
       </c>
-      <c r="B213" s="6">
+      <c r="B213" s="8">
         <v>9.198193035468108E-2</v>
       </c>
       <c r="CG213" s="1"/>
@@ -14990,10 +15005,10 @@
       <c r="RX213" s="1"/>
     </row>
     <row r="214" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A214" s="5">
+      <c r="A214" s="7">
         <v>41122</v>
       </c>
-      <c r="B214" s="6">
+      <c r="B214" s="8">
         <v>9.0527591621574741E-2</v>
       </c>
       <c r="CG214" s="1"/>
@@ -15084,10 +15099,10 @@
       <c r="RX214" s="1"/>
     </row>
     <row r="215" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A215" s="5">
+      <c r="A215" s="7">
         <v>41153</v>
       </c>
-      <c r="B215" s="6">
+      <c r="B215" s="8">
         <v>9.321029129473013E-2</v>
       </c>
       <c r="CG215" s="1"/>
@@ -15164,7 +15179,7 @@
       <c r="PJ215" s="1"/>
       <c r="PU215" s="1"/>
       <c r="PV215" s="1"/>
-      <c r="PW215" s="3"/>
+      <c r="PW215" s="5"/>
       <c r="PX215" s="1"/>
       <c r="PY215" s="1"/>
       <c r="PZ215" s="1"/>
@@ -15178,10 +15193,10 @@
       <c r="RX215" s="1"/>
     </row>
     <row r="216" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A216" s="5">
+      <c r="A216" s="7">
         <v>41183</v>
       </c>
-      <c r="B216" s="6">
+      <c r="B216" s="8">
         <v>9.2447998465240086E-2</v>
       </c>
       <c r="CG216" s="1"/>
@@ -15266,17 +15281,17 @@
       <c r="QB216" s="1"/>
       <c r="QC216" s="1"/>
       <c r="QD216" s="1"/>
-      <c r="QH216" s="3"/>
+      <c r="QH216" s="5"/>
       <c r="QQ216" s="1"/>
       <c r="RB216" s="1"/>
       <c r="RM216" s="1"/>
       <c r="RX216" s="1"/>
     </row>
     <row r="217" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A217" s="5">
+      <c r="A217" s="7">
         <v>41214</v>
       </c>
-      <c r="B217" s="6">
+      <c r="B217" s="8">
         <v>9.5606034425374312E-2</v>
       </c>
       <c r="CG217" s="1"/>
@@ -15367,10 +15382,10 @@
       <c r="RX217" s="1"/>
     </row>
     <row r="218" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A218" s="5">
+      <c r="A218" s="7">
         <v>41244</v>
       </c>
-      <c r="B218" s="6">
+      <c r="B218" s="8">
         <v>9.1047274906739667E-2</v>
       </c>
       <c r="CG218" s="1"/>
@@ -15461,10 +15476,10 @@
       <c r="RX218" s="1"/>
     </row>
     <row r="219" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A219" s="5">
+      <c r="A219" s="7">
         <v>41275</v>
       </c>
-      <c r="B219" s="6">
+      <c r="B219" s="8">
         <v>8.7449844192482862E-2</v>
       </c>
       <c r="CG219" s="1"/>
@@ -15555,10 +15570,10 @@
       <c r="RX219" s="1"/>
     </row>
     <row r="220" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A220" s="5">
+      <c r="A220" s="7">
         <v>41306</v>
       </c>
-      <c r="B220" s="6">
+      <c r="B220" s="8">
         <v>8.9884574591296298E-2</v>
       </c>
       <c r="CG220" s="1"/>
@@ -15649,10 +15664,10 @@
       <c r="RX220" s="1"/>
     </row>
     <row r="221" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A221" s="5">
+      <c r="A221" s="7">
         <v>41334</v>
       </c>
-      <c r="B221" s="6">
+      <c r="B221" s="8">
         <v>8.3440031175367746E-2</v>
       </c>
       <c r="CG221" s="1"/>
@@ -15694,11 +15709,11 @@
       <c r="EJ221" s="1"/>
       <c r="EU221" s="1"/>
       <c r="FF221" s="1"/>
-      <c r="FH221" s="3"/>
+      <c r="FH221" s="5"/>
       <c r="FQ221" s="1"/>
-      <c r="FS221" s="3"/>
+      <c r="FS221" s="5"/>
       <c r="GB221" s="1"/>
-      <c r="GD221" s="3"/>
+      <c r="GD221" s="5"/>
       <c r="GM221" s="1"/>
       <c r="GX221" s="1"/>
       <c r="HI221" s="1"/>
@@ -15746,10 +15761,10 @@
       <c r="RX221" s="1"/>
     </row>
     <row r="222" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A222" s="5">
+      <c r="A222" s="7">
         <v>41365</v>
       </c>
-      <c r="B222" s="6">
+      <c r="B222" s="8">
         <v>8.4749349865796034E-2</v>
       </c>
       <c r="PU222" s="1"/>
@@ -15764,10 +15779,10 @@
       <c r="QD222" s="1"/>
     </row>
     <row r="223" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A223" s="5">
+      <c r="A223" s="7">
         <v>41395</v>
       </c>
-      <c r="B223" s="6">
+      <c r="B223" s="8">
         <v>8.0522617175596833E-2</v>
       </c>
       <c r="PU223" s="1"/>
@@ -15782,10 +15797,10 @@
       <c r="QD223" s="1"/>
     </row>
     <row r="224" spans="1:492" x14ac:dyDescent="0.25">
-      <c r="A224" s="5">
+      <c r="A224" s="7">
         <v>41426</v>
       </c>
-      <c r="B224" s="6">
+      <c r="B224" s="8">
         <v>7.5014888373605801E-2</v>
       </c>
       <c r="PU224" s="1"/>
@@ -15800,10 +15815,10 @@
       <c r="QD224" s="1"/>
     </row>
     <row r="225" spans="1:446" x14ac:dyDescent="0.25">
-      <c r="A225" s="5">
+      <c r="A225" s="7">
         <v>41456</v>
       </c>
-      <c r="B225" s="6">
+      <c r="B225" s="8">
         <v>7.7769653801373628E-2</v>
       </c>
       <c r="PU225" s="1"/>
@@ -15818,10 +15833,10 @@
       <c r="QD225" s="1"/>
     </row>
     <row r="226" spans="1:446" x14ac:dyDescent="0.25">
-      <c r="A226" s="5">
+      <c r="A226" s="7">
         <v>41487</v>
       </c>
-      <c r="B226" s="6">
+      <c r="B226" s="8">
         <v>7.610915084711764E-2</v>
       </c>
       <c r="PU226" s="1"/>
@@ -15836,10 +15851,10 @@
       <c r="QD226" s="1"/>
     </row>
     <row r="227" spans="1:446" x14ac:dyDescent="0.25">
-      <c r="A227" s="5">
+      <c r="A227" s="7">
         <v>41518</v>
       </c>
-      <c r="B227" s="6">
+      <c r="B227" s="8">
         <v>7.4874558269219044E-2</v>
       </c>
       <c r="PU227" s="1"/>
@@ -15854,1000 +15869,1016 @@
       <c r="QD227" s="1"/>
     </row>
     <row r="228" spans="1:446" x14ac:dyDescent="0.25">
-      <c r="A228" s="5">
+      <c r="A228" s="7">
         <v>41548</v>
       </c>
-      <c r="B228" s="6">
+      <c r="B228" s="8">
         <v>7.3769426049519596E-2</v>
       </c>
     </row>
     <row r="229" spans="1:446" x14ac:dyDescent="0.25">
-      <c r="A229" s="5">
+      <c r="A229" s="7">
         <v>41579</v>
       </c>
-      <c r="B229" s="6">
+      <c r="B229" s="8">
         <v>7.9046521727427585E-2</v>
       </c>
     </row>
     <row r="230" spans="1:446" x14ac:dyDescent="0.25">
-      <c r="A230" s="5">
+      <c r="A230" s="7">
         <v>41609</v>
       </c>
-      <c r="B230" s="6">
+      <c r="B230" s="8">
         <v>7.5700418664925911E-2</v>
       </c>
     </row>
     <row r="231" spans="1:446" x14ac:dyDescent="0.25">
-      <c r="A231" s="5">
+      <c r="A231" s="7">
         <v>41640</v>
       </c>
-      <c r="B231" s="6">
+      <c r="B231" s="8">
         <v>8.4845263579311214E-2</v>
       </c>
     </row>
     <row r="232" spans="1:446" x14ac:dyDescent="0.25">
-      <c r="A232" s="5">
+      <c r="A232" s="7">
         <v>41671</v>
       </c>
-      <c r="B232" s="6">
+      <c r="B232" s="8">
         <v>8.4096940621738683E-2</v>
       </c>
     </row>
     <row r="233" spans="1:446" x14ac:dyDescent="0.25">
-      <c r="A233" s="5">
+      <c r="A233" s="7">
         <v>41699</v>
       </c>
-      <c r="B233" s="6">
+      <c r="B233" s="8">
         <v>9.5085723314460191E-2</v>
       </c>
     </row>
     <row r="234" spans="1:446" x14ac:dyDescent="0.25">
-      <c r="A234" s="5">
+      <c r="A234" s="7">
         <v>41730</v>
       </c>
-      <c r="B234" s="6">
+      <c r="B234" s="8">
         <v>9.6617836562715484E-2</v>
       </c>
     </row>
     <row r="235" spans="1:446" x14ac:dyDescent="0.25">
-      <c r="A235" s="5">
+      <c r="A235" s="7">
         <v>41760</v>
       </c>
-      <c r="B235" s="6">
+      <c r="B235" s="8">
         <v>9.8701160485128128E-2</v>
       </c>
     </row>
     <row r="236" spans="1:446" x14ac:dyDescent="0.25">
-      <c r="A236" s="5">
+      <c r="A236" s="7">
         <v>41791</v>
       </c>
-      <c r="B236" s="6">
+      <c r="B236" s="8">
         <v>9.4012780857948633E-2</v>
       </c>
     </row>
     <row r="237" spans="1:446" x14ac:dyDescent="0.25">
-      <c r="A237" s="5">
+      <c r="A237" s="7">
         <v>41821</v>
       </c>
-      <c r="B237" s="6">
+      <c r="B237" s="8">
         <v>9.5099368892112943E-2</v>
       </c>
     </row>
     <row r="238" spans="1:446" x14ac:dyDescent="0.25">
-      <c r="A238" s="5">
+      <c r="A238" s="7">
         <v>41852</v>
       </c>
-      <c r="B238" s="6">
+      <c r="B238" s="8">
         <v>9.5412122648390635E-2</v>
       </c>
     </row>
     <row r="239" spans="1:446" x14ac:dyDescent="0.25">
-      <c r="A239" s="5">
+      <c r="A239" s="7">
         <v>41883</v>
       </c>
-      <c r="B239" s="6">
+      <c r="B239" s="8">
         <v>8.2926779422991759E-2</v>
       </c>
     </row>
     <row r="240" spans="1:446" x14ac:dyDescent="0.25">
-      <c r="A240" s="5">
+      <c r="A240" s="7">
         <v>41913</v>
       </c>
-      <c r="B240" s="6">
+      <c r="B240" s="8">
         <v>8.7456378540700291E-2</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A241" s="5">
+      <c r="A241" s="7">
         <v>41944</v>
       </c>
-      <c r="B241" s="6">
+      <c r="B241" s="8">
         <v>9.0265236245787389E-2</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A242" s="5">
+      <c r="A242" s="7">
         <v>41974</v>
       </c>
-      <c r="B242" s="6">
+      <c r="B242" s="8">
         <v>9.0600536697358139E-2</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A243" s="5">
+      <c r="A243" s="7">
         <v>42005</v>
       </c>
-      <c r="B243" s="6">
+      <c r="B243" s="8">
         <v>0.10533016732361397</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A244" s="5">
+      <c r="A244" s="7">
         <v>42036</v>
       </c>
-      <c r="B244" s="6">
+      <c r="B244" s="8">
         <v>0.10379332898500528</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A245" s="5">
+      <c r="A245" s="7">
         <v>42064</v>
       </c>
-      <c r="B245" s="6">
+      <c r="B245" s="8">
         <v>0.10646618622058883</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A246" s="5">
+      <c r="A246" s="7">
         <v>42095</v>
       </c>
-      <c r="B246" s="6">
+      <c r="B246" s="8">
         <v>0.10277197692695453</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A247" s="5">
+      <c r="A247" s="7">
         <v>42125</v>
       </c>
-      <c r="B247" s="6">
+      <c r="B247" s="8">
         <v>0.10635981236621354</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A248" s="5">
+      <c r="A248" s="7">
         <v>42156</v>
       </c>
-      <c r="B248" s="6">
+      <c r="B248" s="8">
         <v>0.10243622729858951</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A249" s="5">
+      <c r="A249" s="7">
         <v>42186</v>
       </c>
-      <c r="B249" s="6">
+      <c r="B249" s="8">
         <v>0.10824745812912069</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A250" s="5">
+      <c r="A250" s="7">
         <v>42217</v>
       </c>
-      <c r="B250" s="6">
+      <c r="B250" s="8">
         <v>0.11309406133143306</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A251" s="5">
+      <c r="A251" s="7">
         <v>42248</v>
       </c>
-      <c r="B251" s="6">
+      <c r="B251" s="8">
         <v>9.9532565626062719E-2</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A252" s="5">
+      <c r="A252" s="7">
         <v>42278</v>
       </c>
-      <c r="B252" s="6">
+      <c r="B252" s="8">
         <v>9.7344609070752625E-2</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A253" s="5">
+      <c r="A253" s="7">
         <v>42309</v>
       </c>
-      <c r="B253" s="6">
+      <c r="B253" s="8">
         <v>9.6030564044979047E-2</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A254" s="5">
+      <c r="A254" s="7">
         <v>42339</v>
       </c>
-      <c r="B254" s="6">
+      <c r="B254" s="8">
         <v>9.7946408382498046E-2</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A255" s="5">
+      <c r="A255" s="7">
         <v>42370</v>
       </c>
-      <c r="B255" s="6">
+      <c r="B255" s="8">
         <v>0.10720725243654623</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A256" s="5">
+      <c r="A256" s="7">
         <v>42401</v>
       </c>
-      <c r="B256" s="6">
+      <c r="B256" s="8">
         <v>0.10623913533182294</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A257" s="5">
+      <c r="A257" s="7">
         <v>42430</v>
       </c>
-      <c r="B257" s="6">
+      <c r="B257" s="8">
         <v>9.6613329525373437E-2</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A258" s="5">
+      <c r="A258" s="7">
         <v>42461</v>
       </c>
-      <c r="B258" s="6">
+      <c r="B258" s="8">
         <v>9.07458717712184E-2</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A259" s="5">
+      <c r="A259" s="7">
         <v>42491</v>
       </c>
-      <c r="B259" s="6">
+      <c r="B259" s="8">
         <v>8.1503302413437381E-2</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A260" s="5">
+      <c r="A260" s="7">
         <v>42522</v>
       </c>
-      <c r="B260" s="6">
+      <c r="B260" s="8">
         <v>8.4903302413437381E-2</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A261" s="5">
+      <c r="A261" s="7">
         <v>42552</v>
       </c>
-      <c r="B261" s="6">
+      <c r="B261" s="8">
         <v>7.845432079176308E-2</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A262" s="5">
+      <c r="A262" s="7">
         <v>42583</v>
       </c>
-      <c r="B262" s="6">
+      <c r="B262" s="8">
         <v>7.7005107317431515E-2</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A263" s="5">
+      <c r="A263" s="7">
         <v>42614</v>
       </c>
-      <c r="B263" s="6">
+      <c r="B263" s="8">
         <v>7.9062490141365058E-2</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A264" s="5">
+      <c r="A264" s="7">
         <v>42644</v>
       </c>
-      <c r="B264" s="6">
+      <c r="B264" s="8">
         <v>9.0803823058582978E-2</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A265" s="5">
+      <c r="A265" s="7">
         <v>42675</v>
       </c>
-      <c r="B265" s="6">
+      <c r="B265" s="8">
         <v>8.1366322142554626E-2</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A266" s="5">
+      <c r="A266" s="7">
         <v>42705</v>
       </c>
-      <c r="B266" s="6">
+      <c r="B266" s="8">
         <v>8.5524440182112194E-2</v>
       </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A267" s="5">
+      <c r="A267" s="7">
         <v>42736</v>
       </c>
-      <c r="B267" s="6">
+      <c r="B267" s="8">
         <v>8.3374527020277533E-2</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A268" s="5">
+      <c r="A268" s="7">
         <v>42767</v>
       </c>
-      <c r="B268" s="6">
+      <c r="B268" s="8">
         <v>8.2618737455347563E-2</v>
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A269" s="5">
+      <c r="A269" s="7">
         <v>42795</v>
       </c>
-      <c r="B269" s="6">
+      <c r="B269" s="8">
         <v>8.2301802120567966E-2</v>
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A270" s="5">
+      <c r="A270" s="7">
         <v>42826</v>
       </c>
-      <c r="B270" s="6">
+      <c r="B270" s="8">
         <v>7.9480761202343708E-2</v>
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A271" s="5">
+      <c r="A271" s="7">
         <v>42856</v>
       </c>
-      <c r="B271" s="6">
+      <c r="B271" s="8">
         <v>8.3960752894154167E-2</v>
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A272" s="5">
+      <c r="A272" s="7">
         <v>42887</v>
       </c>
-      <c r="B272" s="6">
+      <c r="B272" s="8">
         <v>8.2181900156117982E-2</v>
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A273" s="5">
+      <c r="A273" s="7">
         <v>42917</v>
       </c>
-      <c r="B273" s="6">
+      <c r="B273" s="8">
         <v>7.8582383645718207E-2</v>
       </c>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A274" s="5">
+      <c r="A274" s="7">
         <v>42948</v>
       </c>
-      <c r="B274" s="6">
+      <c r="B274" s="8">
         <v>7.3514830121311145E-2</v>
       </c>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A275" s="5">
+      <c r="A275" s="7">
         <v>42979</v>
       </c>
-      <c r="B275" s="6">
+      <c r="B275" s="8">
         <v>7.1798584083836187E-2</v>
       </c>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A276" s="5">
+      <c r="A276" s="7">
         <v>43009</v>
       </c>
-      <c r="B276" s="6">
+      <c r="B276" s="8">
         <v>7.0893601810297649E-2</v>
       </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A277" s="5">
+      <c r="A277" s="7">
         <v>43040</v>
       </c>
-      <c r="B277" s="6">
+      <c r="B277" s="8">
         <v>6.1052757033422195E-2</v>
       </c>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A278" s="5">
+      <c r="A278" s="7">
         <v>43070</v>
       </c>
-      <c r="B278" s="6">
+      <c r="B278" s="8">
         <v>6.7122786831106646E-2</v>
       </c>
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A279" s="5">
+      <c r="A279" s="7">
         <v>43101</v>
       </c>
-      <c r="B279" s="6">
+      <c r="B279" s="8">
         <v>5.7519098552337958E-2</v>
       </c>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A280" s="5">
+      <c r="A280" s="7">
         <v>43132</v>
       </c>
-      <c r="B280" s="6">
+      <c r="B280" s="8">
         <v>6.5520472026066215E-2</v>
       </c>
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A281" s="5">
+      <c r="A281" s="7">
         <v>43160</v>
       </c>
-      <c r="B281" s="6">
+      <c r="B281" s="8">
         <v>7.2125770364620007E-2</v>
       </c>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A282" s="5">
+      <c r="A282" s="7">
         <v>43191</v>
       </c>
-      <c r="B282" s="6">
+      <c r="B282" s="8">
         <v>6.4064244291655609E-2</v>
       </c>
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A283" s="5">
+      <c r="A283" s="7">
         <v>43221</v>
       </c>
-      <c r="B283" s="6">
+      <c r="B283" s="8">
         <v>7.1824635819149038E-2</v>
       </c>
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A284" s="5">
+      <c r="A284" s="7">
         <v>43252</v>
       </c>
-      <c r="B284" s="6">
+      <c r="B284" s="8">
         <v>7.9775179773577412E-2</v>
       </c>
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A285" s="5">
+      <c r="A285" s="7">
         <v>43282</v>
       </c>
-      <c r="B285" s="6">
+      <c r="B285" s="8">
         <v>9.1939861515753868E-2</v>
       </c>
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A286" s="5">
+      <c r="A286" s="7">
         <v>43313</v>
       </c>
-      <c r="B286" s="6">
+      <c r="B286" s="8">
         <v>0.10101989540599204</v>
       </c>
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A287" s="5">
+      <c r="A287" s="7">
         <v>43344</v>
       </c>
-      <c r="B287" s="6">
+      <c r="B287" s="8">
         <v>0.10496376393363561</v>
       </c>
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A288" s="5">
+      <c r="A288" s="7">
         <v>43374</v>
       </c>
-      <c r="B288" s="6">
+      <c r="B288" s="8">
         <v>6.866534805367612E-2</v>
       </c>
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A289" s="5">
+      <c r="A289" s="7">
         <v>43405</v>
       </c>
-      <c r="B289" s="6">
+      <c r="B289" s="8">
         <v>7.7599591244769228E-2</v>
       </c>
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A290" s="5">
+      <c r="A290" s="7">
         <v>43435</v>
       </c>
-      <c r="B290" s="6">
+      <c r="B290" s="8">
         <v>7.6296518904752947E-2</v>
       </c>
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A291" s="5">
+      <c r="A291" s="7">
         <v>43466</v>
       </c>
-      <c r="B291" s="6">
+      <c r="B291" s="8">
         <v>7.1150211864005483E-2</v>
       </c>
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A292" s="5">
+      <c r="A292" s="7">
         <v>43497</v>
       </c>
-      <c r="B292" s="6">
+      <c r="B292" s="8">
         <v>7.4978703434071342E-2</v>
       </c>
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A293" s="5">
+      <c r="A293" s="7">
         <v>43525</v>
       </c>
-      <c r="B293" s="6">
+      <c r="B293" s="8">
         <v>8.1082222580664831E-2</v>
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A294" s="5">
+      <c r="A294" s="7">
         <v>43556</v>
       </c>
-      <c r="B294" s="6">
+      <c r="B294" s="8">
         <v>8.0864791172512426E-2</v>
       </c>
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A295" s="5">
+      <c r="A295" s="7">
         <v>43586</v>
       </c>
-      <c r="B295" s="6">
+      <c r="B295" s="8">
         <v>8.7764304038109517E-2</v>
       </c>
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A296" s="5">
+      <c r="A296" s="7">
         <v>43617</v>
       </c>
-      <c r="B296" s="6">
+      <c r="B296" s="8">
         <v>8.5839178787788323E-2</v>
       </c>
     </row>
     <row r="297" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A297" s="5">
+      <c r="A297" s="7">
         <v>43647</v>
       </c>
-      <c r="B297" s="6">
+      <c r="B297" s="8">
         <v>8.9544717916765409E-2</v>
       </c>
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A298" s="5">
+      <c r="A298" s="7">
         <v>43678</v>
       </c>
-      <c r="B298" s="6">
+      <c r="B298" s="8">
         <v>9.687272744274146E-2</v>
       </c>
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A299" s="5">
+      <c r="A299" s="7">
         <v>43709</v>
       </c>
-      <c r="B299" s="6">
+      <c r="B299" s="8">
         <v>9.4565670394992141E-2</v>
       </c>
     </row>
     <row r="300" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A300" s="5">
+      <c r="A300" s="7">
         <v>43739</v>
       </c>
-      <c r="B300" s="6">
+      <c r="B300" s="8">
         <v>9.5998871332297536E-2</v>
       </c>
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A301" s="5">
+      <c r="A301" s="7">
         <v>43770</v>
       </c>
-      <c r="B301" s="6">
+      <c r="B301" s="8">
         <v>9.0410180385752506E-2</v>
       </c>
     </row>
     <row r="302" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A302" s="5">
+      <c r="A302" s="7">
         <v>43800</v>
       </c>
-      <c r="B302" s="6">
+      <c r="B302" s="8">
         <v>8.0346430039285821E-2</v>
       </c>
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A303" s="5">
+      <c r="A303" s="7">
         <v>43831</v>
       </c>
-      <c r="B303" s="6">
+      <c r="B303" s="8">
         <v>8.8138805128154862E-2</v>
       </c>
     </row>
     <row r="304" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A304" s="5">
+      <c r="A304" s="7">
         <v>43862</v>
       </c>
-      <c r="B304" s="6">
+      <c r="B304" s="8">
         <v>9.3984258626188408E-2</v>
       </c>
     </row>
     <row r="305" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A305" s="5">
+      <c r="A305" s="7">
         <v>43891</v>
       </c>
-      <c r="B305" s="6">
+      <c r="B305" s="8">
         <v>0.11444455602995118</v>
       </c>
     </row>
     <row r="306" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A306" s="5">
+      <c r="A306" s="7">
         <v>43922</v>
       </c>
-      <c r="B306" s="6">
+      <c r="B306" s="8">
         <v>0.11883485001315314</v>
       </c>
     </row>
     <row r="307" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A307" s="5">
+      <c r="A307" s="7">
         <v>43952</v>
       </c>
-      <c r="B307" s="6">
+      <c r="B307" s="8">
         <v>0.10802006518576782</v>
       </c>
     </row>
     <row r="308" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A308" s="5">
+      <c r="A308" s="7">
         <v>43983</v>
       </c>
-      <c r="B308" s="6">
+      <c r="B308" s="8">
         <v>0.10150000000000001</v>
       </c>
     </row>
     <row r="309" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A309" s="5">
+      <c r="A309" s="7">
         <v>44013</v>
       </c>
-      <c r="B309" s="6">
+      <c r="B309" s="8">
         <v>0.10394071190796175</v>
       </c>
     </row>
     <row r="310" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A310" s="5">
+      <c r="A310" s="7">
         <v>44044</v>
       </c>
-      <c r="B310" s="6">
+      <c r="B310" s="8">
         <v>9.8747906968658955E-2</v>
       </c>
     </row>
     <row r="311" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A311" s="5">
+      <c r="A311" s="7">
         <v>44075</v>
       </c>
-      <c r="B311" s="6">
+      <c r="B311" s="8">
         <v>0.10280377344670942</v>
       </c>
     </row>
     <row r="312" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A312" s="5">
+      <c r="A312" s="7">
         <v>44105</v>
       </c>
-      <c r="B312" s="6">
+      <c r="B312" s="8">
         <v>0.1003081555378784</v>
       </c>
     </row>
     <row r="313" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A313" s="5">
+      <c r="A313" s="7">
         <v>44136</v>
       </c>
-      <c r="B313" s="6">
+      <c r="B313" s="8">
         <v>9.4781090636132159E-2</v>
       </c>
     </row>
     <row r="314" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A314" s="5">
+      <c r="A314" s="7">
         <v>44166</v>
       </c>
-      <c r="B314" s="6">
+      <c r="B314" s="8">
         <v>9.9688114787269883E-2</v>
       </c>
-      <c r="C314" s="8"/>
+      <c r="C314" s="3"/>
     </row>
     <row r="315" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A315" s="5">
+      <c r="A315" s="7">
         <v>44197</v>
       </c>
-      <c r="B315" s="6">
+      <c r="B315" s="8">
         <v>0.10345953791176479</v>
       </c>
-      <c r="C315" s="8"/>
+      <c r="C315" s="3"/>
     </row>
     <row r="316" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A316" s="5">
+      <c r="A316" s="7">
         <v>44228</v>
       </c>
-      <c r="B316" s="6">
+      <c r="B316" s="8">
         <v>9.9036976535253174E-2</v>
       </c>
-      <c r="C316" s="8"/>
+      <c r="C316" s="3"/>
     </row>
     <row r="317" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A317" s="5">
+      <c r="A317" s="7">
         <v>44256</v>
       </c>
-      <c r="B317" s="6">
+      <c r="B317" s="8">
         <v>0.11202004609682872</v>
       </c>
-      <c r="C317" s="8"/>
+      <c r="C317" s="3"/>
     </row>
     <row r="318" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A318" s="5">
+      <c r="A318" s="7">
         <v>44287</v>
       </c>
-      <c r="B318" s="6">
+      <c r="B318" s="8">
         <v>0.1105</v>
       </c>
-      <c r="C318" s="8"/>
+      <c r="C318" s="3"/>
     </row>
     <row r="319" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A319" s="5">
+      <c r="A319" s="7">
         <v>44317</v>
       </c>
-      <c r="B319" s="6">
+      <c r="B319" s="8">
         <v>0.103756060197642</v>
       </c>
-      <c r="C319" s="8"/>
+      <c r="C319" s="3"/>
     </row>
     <row r="320" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A320" s="5">
+      <c r="A320" s="7">
         <v>44348</v>
       </c>
-      <c r="B320" s="6">
+      <c r="B320" s="8">
         <v>0.11288777024068533</v>
       </c>
-      <c r="C320" s="8"/>
+      <c r="C320" s="3"/>
     </row>
     <row r="321" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A321" s="5">
+      <c r="A321" s="7">
         <v>44378</v>
       </c>
-      <c r="B321" s="6">
+      <c r="B321" s="8">
         <v>0.1217</v>
       </c>
-      <c r="C321" s="8"/>
+      <c r="C321" s="3"/>
     </row>
     <row r="322" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A322" s="5">
+      <c r="A322" s="7">
         <v>44409</v>
       </c>
-      <c r="B322" s="6">
+      <c r="B322" s="8">
         <v>0.11860470570232673</v>
       </c>
-      <c r="C322" s="8"/>
+      <c r="C322" s="3"/>
     </row>
     <row r="323" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A323" s="5">
+      <c r="A323" s="7">
         <v>44440</v>
       </c>
-      <c r="B323" s="6">
+      <c r="B323" s="8">
         <v>0.15321467349306883</v>
       </c>
-      <c r="C323" s="8"/>
+      <c r="C323" s="3"/>
     </row>
     <row r="324" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A324" s="5">
+      <c r="A324" s="7">
         <v>44470</v>
       </c>
-      <c r="B324" s="6">
+      <c r="B324" s="8">
         <v>0.1565</v>
       </c>
-      <c r="C324" s="8"/>
+      <c r="C324" s="3"/>
     </row>
     <row r="325" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A325" s="5">
+      <c r="A325" s="7">
         <v>44501</v>
       </c>
-      <c r="B325" s="6">
+      <c r="B325" s="8">
         <v>0.15480116295464194</v>
       </c>
-      <c r="C325" s="8"/>
+      <c r="C325" s="3"/>
     </row>
     <row r="326" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A326" s="5">
+      <c r="A326" s="7">
         <v>44531</v>
       </c>
-      <c r="B326" s="6">
+      <c r="B326" s="8">
         <v>0.18086975473681763</v>
       </c>
-      <c r="C326" s="8"/>
+      <c r="C326" s="3"/>
     </row>
     <row r="327" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A327" s="5">
+      <c r="A327" s="7">
         <v>44562</v>
       </c>
-      <c r="B327" s="6">
+      <c r="B327" s="8">
         <v>0.15203711549166959</v>
       </c>
-      <c r="C327" s="8"/>
+      <c r="C327" s="3"/>
     </row>
     <row r="328" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A328" s="5">
+      <c r="A328" s="7">
         <v>44593</v>
       </c>
-      <c r="B328" s="6">
+      <c r="B328" s="8">
         <v>0.15045086518646858</v>
       </c>
-      <c r="C328" s="8"/>
+      <c r="C328" s="3"/>
     </row>
     <row r="329" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A329" s="5">
+      <c r="A329" s="7">
         <v>44621</v>
       </c>
-      <c r="B329" s="6">
+      <c r="B329" s="8">
         <v>0.13402699778646815</v>
       </c>
-      <c r="C329" s="8"/>
+      <c r="C329" s="3"/>
     </row>
     <row r="330" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A330" s="5">
+      <c r="A330" s="7">
         <v>44652</v>
       </c>
-      <c r="B330" s="6">
+      <c r="B330" s="8">
         <v>0.13661550466927599</v>
       </c>
-      <c r="C330" s="8"/>
+      <c r="C330" s="3"/>
     </row>
     <row r="331" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A331" s="5">
+      <c r="A331" s="7">
         <v>44682</v>
       </c>
-      <c r="B331" s="6">
+      <c r="B331" s="8">
         <v>0.1321</v>
       </c>
-      <c r="C331" s="8"/>
+      <c r="C331" s="3"/>
     </row>
     <row r="332" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A332" s="5">
+      <c r="A332" s="7">
         <v>44713</v>
       </c>
-      <c r="B332" s="6">
+      <c r="B332" s="8">
         <v>0.16510000000000002</v>
       </c>
-      <c r="C332" s="8"/>
+      <c r="C332" s="3"/>
     </row>
     <row r="333" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A333" s="5">
+      <c r="A333" s="7">
         <v>44743</v>
       </c>
-      <c r="B333" s="6">
+      <c r="B333" s="8">
         <v>0.1585</v>
       </c>
-      <c r="C333" s="8"/>
+      <c r="C333" s="3"/>
     </row>
     <row r="334" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A334" s="5">
+      <c r="A334" s="7">
         <v>44774</v>
       </c>
-      <c r="B334" s="6">
+      <c r="B334" s="8">
         <v>0.1331</v>
       </c>
-      <c r="C334" s="8"/>
+      <c r="C334" s="3"/>
     </row>
     <row r="335" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A335" s="5">
+      <c r="A335" s="7">
         <v>44805</v>
       </c>
-      <c r="B335" s="6">
+      <c r="B335" s="8">
         <v>0.14630000000000001</v>
       </c>
-      <c r="C335" s="8"/>
+      <c r="C335" s="3"/>
     </row>
     <row r="336" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A336" s="5">
+      <c r="A336" s="7">
         <v>44835</v>
       </c>
-      <c r="B336" s="6">
+      <c r="B336" s="8">
         <v>0.1197</v>
       </c>
-      <c r="C336" s="8"/>
+      <c r="C336" s="3"/>
     </row>
     <row r="337" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A337" s="5">
+      <c r="A337" s="7">
         <v>44866</v>
       </c>
-      <c r="B337" s="6">
+      <c r="B337" s="8">
         <v>0.1177</v>
       </c>
-      <c r="C337" s="8"/>
+      <c r="C337" s="3"/>
     </row>
     <row r="338" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A338" s="5">
+      <c r="A338" s="7">
         <v>44896</v>
       </c>
-      <c r="B338" s="6">
+      <c r="B338" s="8">
         <v>0.1172183756433729</v>
       </c>
-      <c r="C338" s="8"/>
+      <c r="C338" s="3"/>
     </row>
     <row r="339" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A339" s="5">
+      <c r="A339" s="7">
         <v>44927</v>
       </c>
-      <c r="B339" s="6">
+      <c r="B339" s="8">
         <v>0.112566</v>
       </c>
-      <c r="C339" s="8"/>
+      <c r="C339" s="3"/>
     </row>
     <row r="340" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A340" s="5">
+      <c r="A340" s="7">
         <v>44958</v>
       </c>
-      <c r="B340" s="6">
+      <c r="B340" s="8">
         <v>0.10406600000000001</v>
       </c>
-      <c r="C340" s="8"/>
+      <c r="C340" s="3"/>
     </row>
     <row r="341" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A341" s="5">
+      <c r="A341" s="7">
         <v>44986</v>
       </c>
-      <c r="B341" s="6">
+      <c r="B341" s="8">
         <v>0.100060632666334</v>
       </c>
-      <c r="C341" s="8"/>
+      <c r="C341" s="3"/>
     </row>
     <row r="342" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A342" s="5">
+      <c r="A342" s="7">
         <v>45017</v>
       </c>
-      <c r="B342" s="6">
+      <c r="B342" s="8">
         <v>9.7161250237506505E-2</v>
       </c>
-      <c r="C342" s="8"/>
+      <c r="C342" s="3"/>
     </row>
     <row r="343" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A343" s="5">
+      <c r="A343" s="7">
         <v>45047</v>
       </c>
-      <c r="B343" s="6">
+      <c r="B343" s="8">
         <v>9.6838061660370997E-2</v>
       </c>
     </row>
     <row r="344" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A344" s="5">
+      <c r="A344" s="7">
         <v>45078</v>
       </c>
-      <c r="B344" s="6">
+      <c r="B344" s="8">
         <v>8.4097029271563706E-2</v>
       </c>
-      <c r="C344" s="8"/>
+      <c r="C344" s="3"/>
     </row>
     <row r="345" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A345" s="5">
+      <c r="A345" s="7">
         <v>45108</v>
       </c>
-      <c r="B345" s="6">
+      <c r="B345" s="8">
         <v>7.9421854001553702E-2</v>
       </c>
     </row>
     <row r="346" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A346" s="5">
+      <c r="A346" s="7">
         <v>45139</v>
       </c>
-      <c r="B346" s="6">
+      <c r="B346" s="8">
         <v>8.8703735811575105E-2</v>
       </c>
-      <c r="D346" s="10"/>
+      <c r="D346" s="3"/>
     </row>
     <row r="347" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A347" s="9"/>
+      <c r="A347" s="7">
+        <v>45170</v>
+      </c>
+      <c r="B347" s="8">
+        <v>8.69610556503468E-2</v>
+      </c>
     </row>
     <row r="348" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A348" s="9"/>
+      <c r="A348" s="7">
+        <v>45200</v>
+      </c>
+      <c r="B348" s="8">
+        <v>8.5154952330852907E-2</v>
+      </c>
+      <c r="C348" s="10"/>
     </row>
     <row r="349" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A349" s="9"/>
+      <c r="A349" s="2"/>
     </row>
   </sheetData>
+  <autoFilter ref="A2:B2" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:B348">
+      <sortCondition ref="A2"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Review 2024-08 and script hitorico
</commit_message>
<xml_diff>
--- a/Database/Serie de Equity Risk Premium.xlsx
+++ b/Database/Serie de Equity Risk Premium.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bteba\Documents\GitHub\ERP\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C9C5B88-E5DF-4201-B0AA-1A48F4D8B395}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{272B7920-609A-4E27-8ABC-4B1F4FB3477B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -93,7 +93,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -109,6 +109,7 @@
     <xf numFmtId="17" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2384,7 +2385,7 @@
                   <c:v>9.8254086785083294E-2</c:v>
                 </c:pt>
                 <c:pt idx="355">
-                  <c:v>8.7638597939404303E-2</c:v>
+                  <c:v>9.9822265355109505E-2</c:v>
                 </c:pt>
                 <c:pt idx="356">
                   <c:v>8.7638597939404303E-2</c:v>
@@ -3469,9 +3470,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:RX359"/>
+  <dimension ref="A1:RX360"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A318" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A317" workbookViewId="0">
       <selection activeCell="A359" sqref="A359"/>
     </sheetView>
   </sheetViews>
@@ -17310,7 +17311,7 @@
         <v>45505</v>
       </c>
       <c r="B358" s="3">
-        <v>8.7638597939404303E-2</v>
+        <v>9.9822265355109505E-2</v>
       </c>
     </row>
     <row r="359" spans="1:3" x14ac:dyDescent="0.45">
@@ -17320,6 +17321,9 @@
       <c r="B359" s="3">
         <v>8.7638597939404303E-2</v>
       </c>
+    </row>
+    <row r="360" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A360" s="9"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:B2" xr:uid="{00000000-0001-0000-0000-000000000000}">

</xml_diff>